<commit_message>
add 2018 THLDSL vintage to transport_regionalization_master
</commit_message>
<xml_diff>
--- a/data_aggregation/transport/transport_regionalization_master.xlsx
+++ b/data_aggregation/transport/transport_regionalization_master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiejordan/Documents/GitHub/kathjordan_oeo/data_aggregation/transport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiejordan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7564BE12-A6E7-5649-9E85-3FF6FE13DFF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F28A2B7-E596-7649-80CA-FDBB822AE7CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30580" yWindow="-40" windowWidth="24500" windowHeight="16360" xr2:uid="{E784C07B-F067-AC4C-95FD-EC182FDC45A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22420" windowHeight="17500" activeTab="1" xr2:uid="{E784C07B-F067-AC4C-95FD-EC182FDC45A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand" sheetId="3" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="EmissionActivity" sheetId="7" r:id="rId3"/>
     <sheet name="LifetimeTech" sheetId="9" r:id="rId4"/>
     <sheet name="Efficiency" sheetId="2" r:id="rId5"/>
-    <sheet name="TechInputSplit" sheetId="4" r:id="rId6"/>
-    <sheet name="technologies" sheetId="5" r:id="rId7"/>
-    <sheet name="tech_annual" sheetId="6" r:id="rId8"/>
-    <sheet name="needs deleting" sheetId="8" r:id="rId9"/>
+    <sheet name="CostVariable" sheetId="10" r:id="rId6"/>
+    <sheet name="TechInputSplit" sheetId="4" r:id="rId7"/>
+    <sheet name="technologies" sheetId="5" r:id="rId8"/>
+    <sheet name="tech_annual" sheetId="6" r:id="rId9"/>
+    <sheet name="needs deleting" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Demand!$A$1:$F$743</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Efficiency!$A$1:$G$82</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EmissionActivity!$A$1:$I$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EmissionActivity!$A$1:$I$136</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ExistingCapacity!$B$1:$B$1469</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5" concurrentCalc="0"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13933" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14462" uniqueCount="207">
   <si>
     <t>regions</t>
   </si>
@@ -642,6 +643,33 @@
   <si>
     <t>ELC_TRN</t>
   </si>
+  <si>
+    <t>DSL</t>
+  </si>
+  <si>
+    <t>TMDHDV_HTL_DSL</t>
+  </si>
+  <si>
+    <t>#VT_EPAUS9rT_TRNHDV_v18.1.1full.xlsx, TechData_HDV_EMIS</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy21osti/71796.pdf figure 25</t>
+  </si>
+  <si>
+    <t>M$/bvmt</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy21osti/71796.pdf table 5</t>
+  </si>
+  <si>
+    <t>cost_variable</t>
+  </si>
+  <si>
+    <t>cost_variable_units</t>
+  </si>
+  <si>
+    <t>cost_variable_notes</t>
+  </si>
 </sst>
 </file>
 
@@ -1020,7 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5BAA25-0133-4242-BE9A-4343197BBF61}">
   <dimension ref="A1:F743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H161" sqref="H161"/>
     </sheetView>
   </sheetViews>
@@ -15710,13 +15738,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E93042-7294-BF4C-AE0A-DBD708DEC29E}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90557C9-C767-8C4E-81AD-DC2D04727A3B}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G1469"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E680" sqref="E680"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1418" sqref="D1418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15746,7 +15889,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" hidden="1">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -15872,7 +16015,7 @@
       </c>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" hidden="1">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -16081,7 +16224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:6" customFormat="1">
+    <row r="18" spans="1:6" customFormat="1" hidden="1">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -16181,7 +16324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" customFormat="1">
+    <row r="23" spans="1:6" customFormat="1" hidden="1">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -16361,7 +16504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:6" customFormat="1">
+    <row r="32" spans="1:6" customFormat="1" hidden="1">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -16481,7 +16624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" customFormat="1">
+    <row r="38" spans="1:6" customFormat="1" hidden="1">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -16681,7 +16824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:6" customFormat="1">
+    <row r="48" spans="1:6" customFormat="1" hidden="1">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -16781,7 +16924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:6" customFormat="1">
+    <row r="53" spans="1:6" customFormat="1" hidden="1">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -16961,7 +17104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:6" customFormat="1">
+    <row r="62" spans="1:6" customFormat="1" hidden="1">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -17081,7 +17224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:6" customFormat="1">
+    <row r="68" spans="1:6" customFormat="1" hidden="1">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -17281,7 +17424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="78" spans="1:6" customFormat="1">
+    <row r="78" spans="1:6" customFormat="1" hidden="1">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -17381,7 +17524,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:6" customFormat="1">
+    <row r="83" spans="1:6" customFormat="1" hidden="1">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -17561,7 +17704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:6" customFormat="1">
+    <row r="92" spans="1:6" customFormat="1" hidden="1">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -17681,7 +17824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="1:6" customFormat="1">
+    <row r="98" spans="1:6" customFormat="1" hidden="1">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -17881,7 +18024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="108" spans="1:6" customFormat="1">
+    <row r="108" spans="1:6" customFormat="1" hidden="1">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -17981,7 +18124,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:6" customFormat="1">
+    <row r="113" spans="1:6" customFormat="1" hidden="1">
       <c r="A113" t="s">
         <v>12</v>
       </c>
@@ -18161,7 +18304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="122" spans="1:6" customFormat="1">
+    <row r="122" spans="1:6" customFormat="1" hidden="1">
       <c r="A122" t="s">
         <v>13</v>
       </c>
@@ -18281,7 +18424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="1:6" customFormat="1">
+    <row r="128" spans="1:6" customFormat="1" hidden="1">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -18481,7 +18624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="138" spans="1:6" customFormat="1">
+    <row r="138" spans="1:6" customFormat="1" hidden="1">
       <c r="A138" t="s">
         <v>13</v>
       </c>
@@ -18581,7 +18724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="143" spans="1:6" customFormat="1">
+    <row r="143" spans="1:6" customFormat="1" hidden="1">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -18761,7 +18904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:6" customFormat="1">
+    <row r="152" spans="1:6" customFormat="1" hidden="1">
       <c r="A152" t="s">
         <v>14</v>
       </c>
@@ -18881,7 +19024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="158" spans="1:6" customFormat="1">
+    <row r="158" spans="1:6" customFormat="1" hidden="1">
       <c r="A158" t="s">
         <v>14</v>
       </c>
@@ -19081,7 +19224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:6" customFormat="1">
+    <row r="168" spans="1:6" customFormat="1" hidden="1">
       <c r="A168" t="s">
         <v>14</v>
       </c>
@@ -19181,7 +19324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:6" customFormat="1">
+    <row r="173" spans="1:6" customFormat="1" hidden="1">
       <c r="A173" t="s">
         <v>14</v>
       </c>
@@ -19361,7 +19504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:6" customFormat="1">
+    <row r="182" spans="1:6" customFormat="1" hidden="1">
       <c r="A182" t="s">
         <v>15</v>
       </c>
@@ -19481,7 +19624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:6" customFormat="1">
+    <row r="188" spans="1:6" customFormat="1" hidden="1">
       <c r="A188" t="s">
         <v>15</v>
       </c>
@@ -19681,7 +19824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:6" customFormat="1">
+    <row r="198" spans="1:6" customFormat="1" hidden="1">
       <c r="A198" t="s">
         <v>15</v>
       </c>
@@ -19781,7 +19924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:6" customFormat="1">
+    <row r="203" spans="1:6" customFormat="1" hidden="1">
       <c r="A203" t="s">
         <v>15</v>
       </c>
@@ -19961,7 +20104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="212" spans="1:6" customFormat="1">
+    <row r="212" spans="1:6" customFormat="1" hidden="1">
       <c r="A212" t="s">
         <v>16</v>
       </c>
@@ -20081,7 +20224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="218" spans="1:6" customFormat="1">
+    <row r="218" spans="1:6" customFormat="1" hidden="1">
       <c r="A218" t="s">
         <v>16</v>
       </c>
@@ -20281,7 +20424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="228" spans="1:6" customFormat="1">
+    <row r="228" spans="1:6" customFormat="1" hidden="1">
       <c r="A228" t="s">
         <v>16</v>
       </c>
@@ -20381,7 +20524,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:6" customFormat="1">
+    <row r="233" spans="1:6" customFormat="1" hidden="1">
       <c r="A233" t="s">
         <v>16</v>
       </c>
@@ -20561,7 +20704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="242" spans="1:6" customFormat="1">
+    <row r="242" spans="1:6" customFormat="1" hidden="1">
       <c r="A242" t="s">
         <v>17</v>
       </c>
@@ -20681,7 +20824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="248" spans="1:6" customFormat="1">
+    <row r="248" spans="1:6" customFormat="1" hidden="1">
       <c r="A248" t="s">
         <v>17</v>
       </c>
@@ -20881,7 +21024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="258" spans="1:6" customFormat="1">
+    <row r="258" spans="1:6" customFormat="1" hidden="1">
       <c r="A258" t="s">
         <v>17</v>
       </c>
@@ -20981,7 +21124,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="263" spans="1:6" customFormat="1">
+    <row r="263" spans="1:6" customFormat="1" hidden="1">
       <c r="A263" t="s">
         <v>17</v>
       </c>
@@ -21161,7 +21304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="272" spans="1:6" customFormat="1">
+    <row r="272" spans="1:6" customFormat="1" hidden="1">
       <c r="A272" t="s">
         <v>6</v>
       </c>
@@ -21281,7 +21424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="278" spans="1:6" customFormat="1">
+    <row r="278" spans="1:6" customFormat="1" hidden="1">
       <c r="A278" t="s">
         <v>6</v>
       </c>
@@ -21481,7 +21624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="288" spans="1:6" customFormat="1">
+    <row r="288" spans="1:6" customFormat="1" hidden="1">
       <c r="A288" t="s">
         <v>6</v>
       </c>
@@ -21581,7 +21724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="293" spans="1:6" customFormat="1">
+    <row r="293" spans="1:6" customFormat="1" hidden="1">
       <c r="A293" t="s">
         <v>6</v>
       </c>
@@ -21761,7 +21904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="302" spans="1:6" customFormat="1">
+    <row r="302" spans="1:6" customFormat="1" hidden="1">
       <c r="A302" t="s">
         <v>10</v>
       </c>
@@ -21881,7 +22024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="308" spans="1:6" customFormat="1">
+    <row r="308" spans="1:6" customFormat="1" hidden="1">
       <c r="A308" t="s">
         <v>10</v>
       </c>
@@ -22081,7 +22224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="318" spans="1:6" customFormat="1">
+    <row r="318" spans="1:6" customFormat="1" hidden="1">
       <c r="A318" t="s">
         <v>10</v>
       </c>
@@ -22181,7 +22324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="323" spans="1:6" customFormat="1">
+    <row r="323" spans="1:6" customFormat="1" hidden="1">
       <c r="A323" t="s">
         <v>10</v>
       </c>
@@ -22361,7 +22504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="332" spans="1:6" customFormat="1">
+    <row r="332" spans="1:6" customFormat="1" hidden="1">
       <c r="A332" t="s">
         <v>11</v>
       </c>
@@ -22481,7 +22624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="338" spans="1:6" customFormat="1">
+    <row r="338" spans="1:6" customFormat="1" hidden="1">
       <c r="A338" t="s">
         <v>11</v>
       </c>
@@ -22681,7 +22824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="348" spans="1:6" customFormat="1">
+    <row r="348" spans="1:6" customFormat="1" hidden="1">
       <c r="A348" t="s">
         <v>11</v>
       </c>
@@ -22781,7 +22924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="353" spans="1:6" customFormat="1">
+    <row r="353" spans="1:6" customFormat="1" hidden="1">
       <c r="A353" t="s">
         <v>11</v>
       </c>
@@ -22961,7 +23104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="362" spans="1:6" customFormat="1">
+    <row r="362" spans="1:6" customFormat="1" hidden="1">
       <c r="A362" t="s">
         <v>12</v>
       </c>
@@ -23081,7 +23224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="368" spans="1:6" customFormat="1">
+    <row r="368" spans="1:6" customFormat="1" hidden="1">
       <c r="A368" t="s">
         <v>12</v>
       </c>
@@ -23281,7 +23424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="378" spans="1:6" customFormat="1">
+    <row r="378" spans="1:6" customFormat="1" hidden="1">
       <c r="A378" t="s">
         <v>12</v>
       </c>
@@ -23381,7 +23524,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="383" spans="1:6" customFormat="1">
+    <row r="383" spans="1:6" customFormat="1" hidden="1">
       <c r="A383" t="s">
         <v>12</v>
       </c>
@@ -23561,7 +23704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="392" spans="1:6" customFormat="1">
+    <row r="392" spans="1:6" customFormat="1" hidden="1">
       <c r="A392" t="s">
         <v>13</v>
       </c>
@@ -23681,7 +23824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="398" spans="1:6" customFormat="1">
+    <row r="398" spans="1:6" customFormat="1" hidden="1">
       <c r="A398" t="s">
         <v>13</v>
       </c>
@@ -23881,7 +24024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="408" spans="1:6" customFormat="1">
+    <row r="408" spans="1:6" customFormat="1" hidden="1">
       <c r="A408" t="s">
         <v>13</v>
       </c>
@@ -23981,7 +24124,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="413" spans="1:6" customFormat="1">
+    <row r="413" spans="1:6" customFormat="1" hidden="1">
       <c r="A413" t="s">
         <v>13</v>
       </c>
@@ -24161,7 +24304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="422" spans="1:6" customFormat="1">
+    <row r="422" spans="1:6" customFormat="1" hidden="1">
       <c r="A422" t="s">
         <v>14</v>
       </c>
@@ -24281,7 +24424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="428" spans="1:6" customFormat="1">
+    <row r="428" spans="1:6" customFormat="1" hidden="1">
       <c r="A428" t="s">
         <v>14</v>
       </c>
@@ -24481,7 +24624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="438" spans="1:6" customFormat="1">
+    <row r="438" spans="1:6" customFormat="1" hidden="1">
       <c r="A438" t="s">
         <v>14</v>
       </c>
@@ -24581,7 +24724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="443" spans="1:6" customFormat="1">
+    <row r="443" spans="1:6" customFormat="1" hidden="1">
       <c r="A443" t="s">
         <v>14</v>
       </c>
@@ -24761,7 +24904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="452" spans="1:6" customFormat="1">
+    <row r="452" spans="1:6" customFormat="1" hidden="1">
       <c r="A452" t="s">
         <v>15</v>
       </c>
@@ -24881,7 +25024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="458" spans="1:6" customFormat="1">
+    <row r="458" spans="1:6" customFormat="1" hidden="1">
       <c r="A458" t="s">
         <v>15</v>
       </c>
@@ -25081,7 +25224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="468" spans="1:6" customFormat="1">
+    <row r="468" spans="1:6" customFormat="1" hidden="1">
       <c r="A468" t="s">
         <v>15</v>
       </c>
@@ -25181,7 +25324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="473" spans="1:6" customFormat="1">
+    <row r="473" spans="1:6" customFormat="1" hidden="1">
       <c r="A473" t="s">
         <v>15</v>
       </c>
@@ -25361,7 +25504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="482" spans="1:6" customFormat="1">
+    <row r="482" spans="1:6" customFormat="1" hidden="1">
       <c r="A482" t="s">
         <v>16</v>
       </c>
@@ -25481,7 +25624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="488" spans="1:6" customFormat="1">
+    <row r="488" spans="1:6" customFormat="1" hidden="1">
       <c r="A488" t="s">
         <v>16</v>
       </c>
@@ -25681,7 +25824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="498" spans="1:6" customFormat="1">
+    <row r="498" spans="1:6" customFormat="1" hidden="1">
       <c r="A498" t="s">
         <v>16</v>
       </c>
@@ -25781,7 +25924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="503" spans="1:6" customFormat="1">
+    <row r="503" spans="1:6" customFormat="1" hidden="1">
       <c r="A503" t="s">
         <v>16</v>
       </c>
@@ -25961,7 +26104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="512" spans="1:6" customFormat="1">
+    <row r="512" spans="1:6" customFormat="1" hidden="1">
       <c r="A512" t="s">
         <v>17</v>
       </c>
@@ -26081,7 +26224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="518" spans="1:6" customFormat="1">
+    <row r="518" spans="1:6" customFormat="1" hidden="1">
       <c r="A518" t="s">
         <v>17</v>
       </c>
@@ -26281,7 +26424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="528" spans="1:6" customFormat="1">
+    <row r="528" spans="1:6" customFormat="1" hidden="1">
       <c r="A528" t="s">
         <v>17</v>
       </c>
@@ -26385,7 +26528,7 @@
       </c>
       <c r="G532"/>
     </row>
-    <row r="533" spans="1:7">
+    <row r="533" spans="1:7" hidden="1">
       <c r="A533" t="s">
         <v>17</v>
       </c>
@@ -26574,7 +26717,7 @@
       </c>
       <c r="G541"/>
     </row>
-    <row r="542" spans="1:7">
+    <row r="542" spans="1:7" hidden="1">
       <c r="A542" t="s">
         <v>6</v>
       </c>
@@ -26595,7 +26738,7 @@
       </c>
       <c r="G542"/>
     </row>
-    <row r="543" spans="1:7">
+    <row r="543" spans="1:7" hidden="1">
       <c r="A543" t="s">
         <v>10</v>
       </c>
@@ -26616,7 +26759,7 @@
       </c>
       <c r="G543"/>
     </row>
-    <row r="544" spans="1:7">
+    <row r="544" spans="1:7" hidden="1">
       <c r="A544" t="s">
         <v>11</v>
       </c>
@@ -26637,7 +26780,7 @@
       </c>
       <c r="G544"/>
     </row>
-    <row r="545" spans="1:7">
+    <row r="545" spans="1:7" hidden="1">
       <c r="A545" t="s">
         <v>12</v>
       </c>
@@ -26658,7 +26801,7 @@
       </c>
       <c r="G545"/>
     </row>
-    <row r="546" spans="1:7">
+    <row r="546" spans="1:7" hidden="1">
       <c r="A546" t="s">
         <v>13</v>
       </c>
@@ -26679,7 +26822,7 @@
       </c>
       <c r="G546"/>
     </row>
-    <row r="547" spans="1:7">
+    <row r="547" spans="1:7" hidden="1">
       <c r="A547" t="s">
         <v>14</v>
       </c>
@@ -26700,7 +26843,7 @@
       </c>
       <c r="G547"/>
     </row>
-    <row r="548" spans="1:7">
+    <row r="548" spans="1:7" hidden="1">
       <c r="A548" t="s">
         <v>15</v>
       </c>
@@ -26721,7 +26864,7 @@
       </c>
       <c r="G548"/>
     </row>
-    <row r="549" spans="1:7">
+    <row r="549" spans="1:7" hidden="1">
       <c r="A549" t="s">
         <v>16</v>
       </c>
@@ -26742,7 +26885,7 @@
       </c>
       <c r="G549"/>
     </row>
-    <row r="550" spans="1:7">
+    <row r="550" spans="1:7" hidden="1">
       <c r="A550" t="s">
         <v>17</v>
       </c>
@@ -27519,7 +27662,7 @@
       </c>
       <c r="G586"/>
     </row>
-    <row r="587" spans="1:7">
+    <row r="587" spans="1:7" hidden="1">
       <c r="A587" t="s">
         <v>6</v>
       </c>
@@ -27540,7 +27683,7 @@
       </c>
       <c r="G587"/>
     </row>
-    <row r="588" spans="1:7">
+    <row r="588" spans="1:7" hidden="1">
       <c r="A588" t="s">
         <v>10</v>
       </c>
@@ -27561,7 +27704,7 @@
       </c>
       <c r="G588"/>
     </row>
-    <row r="589" spans="1:7">
+    <row r="589" spans="1:7" hidden="1">
       <c r="A589" t="s">
         <v>11</v>
       </c>
@@ -27582,7 +27725,7 @@
       </c>
       <c r="G589"/>
     </row>
-    <row r="590" spans="1:7">
+    <row r="590" spans="1:7" hidden="1">
       <c r="A590" t="s">
         <v>12</v>
       </c>
@@ -27603,7 +27746,7 @@
       </c>
       <c r="G590"/>
     </row>
-    <row r="591" spans="1:7">
+    <row r="591" spans="1:7" hidden="1">
       <c r="A591" t="s">
         <v>13</v>
       </c>
@@ -27624,7 +27767,7 @@
       </c>
       <c r="G591"/>
     </row>
-    <row r="592" spans="1:7">
+    <row r="592" spans="1:7" hidden="1">
       <c r="A592" t="s">
         <v>14</v>
       </c>
@@ -27645,7 +27788,7 @@
       </c>
       <c r="G592"/>
     </row>
-    <row r="593" spans="1:7">
+    <row r="593" spans="1:7" hidden="1">
       <c r="A593" t="s">
         <v>15</v>
       </c>
@@ -27666,7 +27809,7 @@
       </c>
       <c r="G593"/>
     </row>
-    <row r="594" spans="1:7">
+    <row r="594" spans="1:7" hidden="1">
       <c r="A594" t="s">
         <v>16</v>
       </c>
@@ -27687,7 +27830,7 @@
       </c>
       <c r="G594"/>
     </row>
-    <row r="595" spans="1:7">
+    <row r="595" spans="1:7" hidden="1">
       <c r="A595" t="s">
         <v>17</v>
       </c>
@@ -28464,7 +28607,7 @@
       </c>
       <c r="G631"/>
     </row>
-    <row r="632" spans="1:7">
+    <row r="632" spans="1:7" hidden="1">
       <c r="A632" t="s">
         <v>6</v>
       </c>
@@ -28485,7 +28628,7 @@
       </c>
       <c r="G632"/>
     </row>
-    <row r="633" spans="1:7">
+    <row r="633" spans="1:7" hidden="1">
       <c r="A633" t="s">
         <v>10</v>
       </c>
@@ -28506,7 +28649,7 @@
       </c>
       <c r="G633"/>
     </row>
-    <row r="634" spans="1:7">
+    <row r="634" spans="1:7" hidden="1">
       <c r="A634" t="s">
         <v>11</v>
       </c>
@@ -28527,7 +28670,7 @@
       </c>
       <c r="G634"/>
     </row>
-    <row r="635" spans="1:7">
+    <row r="635" spans="1:7" hidden="1">
       <c r="A635" t="s">
         <v>12</v>
       </c>
@@ -28548,7 +28691,7 @@
       </c>
       <c r="G635"/>
     </row>
-    <row r="636" spans="1:7">
+    <row r="636" spans="1:7" hidden="1">
       <c r="A636" t="s">
         <v>13</v>
       </c>
@@ -28569,7 +28712,7 @@
       </c>
       <c r="G636"/>
     </row>
-    <row r="637" spans="1:7">
+    <row r="637" spans="1:7" hidden="1">
       <c r="A637" t="s">
         <v>14</v>
       </c>
@@ -28590,7 +28733,7 @@
       </c>
       <c r="G637"/>
     </row>
-    <row r="638" spans="1:7">
+    <row r="638" spans="1:7" hidden="1">
       <c r="A638" t="s">
         <v>15</v>
       </c>
@@ -28611,7 +28754,7 @@
       </c>
       <c r="G638"/>
     </row>
-    <row r="639" spans="1:7">
+    <row r="639" spans="1:7" hidden="1">
       <c r="A639" t="s">
         <v>16</v>
       </c>
@@ -28632,7 +28775,7 @@
       </c>
       <c r="G639"/>
     </row>
-    <row r="640" spans="1:7">
+    <row r="640" spans="1:7" hidden="1">
       <c r="A640" t="s">
         <v>17</v>
       </c>
@@ -29419,7 +29562,7 @@
       <c r="C677" s="5">
         <v>2005</v>
       </c>
-      <c r="D677" s="5">
+      <c r="D677">
         <v>2.8274137896900702</v>
       </c>
       <c r="E677" s="5" t="s">
@@ -29439,7 +29582,7 @@
       <c r="C678" s="5">
         <v>2010</v>
       </c>
-      <c r="D678" s="5">
+      <c r="D678">
         <v>2.8274137896900702</v>
       </c>
       <c r="E678" s="5" t="s">
@@ -29459,7 +29602,7 @@
       <c r="C679" s="5">
         <v>2015</v>
       </c>
-      <c r="D679" s="5">
+      <c r="D679">
         <v>2.8274137896900702</v>
       </c>
       <c r="E679" s="5" t="s">
@@ -29479,7 +29622,7 @@
       <c r="C680" s="5">
         <v>2005</v>
       </c>
-      <c r="D680" s="5">
+      <c r="D680">
         <v>3.4639106615238799</v>
       </c>
       <c r="E680" s="5" t="s">
@@ -29499,7 +29642,7 @@
       <c r="C681" s="5">
         <v>2010</v>
       </c>
-      <c r="D681" s="5">
+      <c r="D681">
         <v>3.4639106615238799</v>
       </c>
       <c r="E681" s="5" t="s">
@@ -29519,7 +29662,7 @@
       <c r="C682" s="5">
         <v>2015</v>
       </c>
-      <c r="D682" s="5">
+      <c r="D682">
         <v>3.4639106615238799</v>
       </c>
       <c r="E682" s="5" t="s">
@@ -29539,7 +29682,7 @@
       <c r="C683" s="5">
         <v>2005</v>
       </c>
-      <c r="D683" s="5">
+      <c r="D683">
         <v>3.5266421098875802</v>
       </c>
       <c r="E683" s="5" t="s">
@@ -29559,7 +29702,7 @@
       <c r="C684" s="5">
         <v>2010</v>
       </c>
-      <c r="D684" s="5">
+      <c r="D684">
         <v>3.5266421098875802</v>
       </c>
       <c r="E684" s="5" t="s">
@@ -29579,7 +29722,7 @@
       <c r="C685" s="5">
         <v>2015</v>
       </c>
-      <c r="D685" s="5">
+      <c r="D685">
         <v>3.5266421098875802</v>
       </c>
       <c r="E685" s="5" t="s">
@@ -29599,7 +29742,7 @@
       <c r="C686" s="5">
         <v>2005</v>
       </c>
-      <c r="D686" s="5">
+      <c r="D686">
         <v>1.39135059941274</v>
       </c>
       <c r="E686" s="5" t="s">
@@ -29619,7 +29762,7 @@
       <c r="C687" s="5">
         <v>2010</v>
       </c>
-      <c r="D687" s="5">
+      <c r="D687">
         <v>1.39135059941274</v>
       </c>
       <c r="E687" s="5" t="s">
@@ -29639,7 +29782,7 @@
       <c r="C688" s="5">
         <v>2015</v>
       </c>
-      <c r="D688" s="5">
+      <c r="D688">
         <v>1.39135059941274</v>
       </c>
       <c r="E688" s="5" t="s">
@@ -29659,7 +29802,7 @@
       <c r="C689" s="5">
         <v>2005</v>
       </c>
-      <c r="D689" s="5">
+      <c r="D689">
         <v>1.2151303931116899</v>
       </c>
       <c r="E689" s="5" t="s">
@@ -29679,7 +29822,7 @@
       <c r="C690" s="5">
         <v>2010</v>
       </c>
-      <c r="D690" s="5">
+      <c r="D690">
         <v>1.2151303931116899</v>
       </c>
       <c r="E690" s="5" t="s">
@@ -29699,7 +29842,7 @@
       <c r="C691" s="5">
         <v>2015</v>
       </c>
-      <c r="D691" s="5">
+      <c r="D691">
         <v>1.2151303931116899</v>
       </c>
       <c r="E691" s="5" t="s">
@@ -29719,7 +29862,7 @@
       <c r="C692" s="5">
         <v>2005</v>
       </c>
-      <c r="D692" s="5">
+      <c r="D692">
         <v>4.1872025601742902</v>
       </c>
       <c r="E692" s="5" t="s">
@@ -29739,7 +29882,7 @@
       <c r="C693" s="5">
         <v>2010</v>
       </c>
-      <c r="D693" s="5">
+      <c r="D693">
         <v>4.1872025601742902</v>
       </c>
       <c r="E693" s="5" t="s">
@@ -29759,7 +29902,7 @@
       <c r="C694" s="5">
         <v>2015</v>
       </c>
-      <c r="D694" s="5">
+      <c r="D694">
         <v>4.1872025601742902</v>
       </c>
       <c r="E694" s="5" t="s">
@@ -29779,7 +29922,7 @@
       <c r="C695" s="5">
         <v>2005</v>
       </c>
-      <c r="D695" s="5">
+      <c r="D695">
         <v>5.73110199299831</v>
       </c>
       <c r="E695" s="5" t="s">
@@ -29799,7 +29942,7 @@
       <c r="C696" s="5">
         <v>2010</v>
       </c>
-      <c r="D696" s="5">
+      <c r="D696">
         <v>5.73110199299831</v>
       </c>
       <c r="E696" s="5" t="s">
@@ -29819,7 +29962,7 @@
       <c r="C697" s="5">
         <v>2015</v>
       </c>
-      <c r="D697" s="5">
+      <c r="D697">
         <v>5.73110199299831</v>
       </c>
       <c r="E697" s="5" t="s">
@@ -29839,7 +29982,7 @@
       <c r="C698" s="5">
         <v>2005</v>
       </c>
-      <c r="D698" s="5">
+      <c r="D698">
         <v>1.9515730522953301</v>
       </c>
       <c r="E698" s="5" t="s">
@@ -29859,7 +30002,7 @@
       <c r="C699" s="5">
         <v>2010</v>
       </c>
-      <c r="D699" s="5">
+      <c r="D699">
         <v>1.9515730522953301</v>
       </c>
       <c r="E699" s="5" t="s">
@@ -29879,7 +30022,7 @@
       <c r="C700" s="5">
         <v>2015</v>
       </c>
-      <c r="D700" s="5">
+      <c r="D700">
         <v>1.9515730522953301</v>
       </c>
       <c r="E700" s="5" t="s">
@@ -29899,7 +30042,7 @@
       <c r="C701" s="5">
         <v>2005</v>
       </c>
-      <c r="D701" s="5">
+      <c r="D701">
         <v>3.7006243651556199</v>
       </c>
       <c r="E701" s="5" t="s">
@@ -29919,7 +30062,7 @@
       <c r="C702" s="5">
         <v>2010</v>
       </c>
-      <c r="D702" s="5">
+      <c r="D702">
         <v>3.7006243651556199</v>
       </c>
       <c r="E702" s="5" t="s">
@@ -29939,7 +30082,7 @@
       <c r="C703" s="5">
         <v>2015</v>
       </c>
-      <c r="D703" s="5">
+      <c r="D703">
         <v>3.7006243651556199</v>
       </c>
       <c r="E703" s="5" t="s">
@@ -30003,7 +30146,7 @@
     <row r="721" spans="1:7" hidden="1">
       <c r="G721"/>
     </row>
-    <row r="722" spans="1:7">
+    <row r="722" spans="1:7" hidden="1">
       <c r="A722" t="s">
         <v>6</v>
       </c>
@@ -30024,7 +30167,7 @@
       </c>
       <c r="G722"/>
     </row>
-    <row r="723" spans="1:7">
+    <row r="723" spans="1:7" hidden="1">
       <c r="A723" t="s">
         <v>10</v>
       </c>
@@ -30045,7 +30188,7 @@
       </c>
       <c r="G723"/>
     </row>
-    <row r="724" spans="1:7">
+    <row r="724" spans="1:7" hidden="1">
       <c r="A724" t="s">
         <v>11</v>
       </c>
@@ -30066,7 +30209,7 @@
       </c>
       <c r="G724"/>
     </row>
-    <row r="725" spans="1:7">
+    <row r="725" spans="1:7" hidden="1">
       <c r="A725" t="s">
         <v>12</v>
       </c>
@@ -30087,7 +30230,7 @@
       </c>
       <c r="G725"/>
     </row>
-    <row r="726" spans="1:7">
+    <row r="726" spans="1:7" hidden="1">
       <c r="A726" t="s">
         <v>13</v>
       </c>
@@ -30108,7 +30251,7 @@
       </c>
       <c r="G726"/>
     </row>
-    <row r="727" spans="1:7">
+    <row r="727" spans="1:7" hidden="1">
       <c r="A727" t="s">
         <v>14</v>
       </c>
@@ -30129,7 +30272,7 @@
       </c>
       <c r="G727"/>
     </row>
-    <row r="728" spans="1:7">
+    <row r="728" spans="1:7" hidden="1">
       <c r="A728" t="s">
         <v>15</v>
       </c>
@@ -30150,7 +30293,7 @@
       </c>
       <c r="G728"/>
     </row>
-    <row r="729" spans="1:7">
+    <row r="729" spans="1:7" hidden="1">
       <c r="A729" t="s">
         <v>16</v>
       </c>
@@ -30171,7 +30314,7 @@
       </c>
       <c r="G729"/>
     </row>
-    <row r="730" spans="1:7">
+    <row r="730" spans="1:7" hidden="1">
       <c r="A730" t="s">
         <v>17</v>
       </c>
@@ -30759,7 +30902,7 @@
       </c>
       <c r="G757"/>
     </row>
-    <row r="758" spans="1:7">
+    <row r="758" spans="1:7" hidden="1">
       <c r="A758" t="s">
         <v>6</v>
       </c>
@@ -30780,7 +30923,7 @@
       </c>
       <c r="G758"/>
     </row>
-    <row r="759" spans="1:7">
+    <row r="759" spans="1:7" hidden="1">
       <c r="A759" t="s">
         <v>10</v>
       </c>
@@ -30801,7 +30944,7 @@
       </c>
       <c r="G759"/>
     </row>
-    <row r="760" spans="1:7">
+    <row r="760" spans="1:7" hidden="1">
       <c r="A760" t="s">
         <v>11</v>
       </c>
@@ -30822,7 +30965,7 @@
       </c>
       <c r="G760"/>
     </row>
-    <row r="761" spans="1:7">
+    <row r="761" spans="1:7" hidden="1">
       <c r="A761" t="s">
         <v>12</v>
       </c>
@@ -30843,7 +30986,7 @@
       </c>
       <c r="G761"/>
     </row>
-    <row r="762" spans="1:7">
+    <row r="762" spans="1:7" hidden="1">
       <c r="A762" t="s">
         <v>13</v>
       </c>
@@ -30864,7 +31007,7 @@
       </c>
       <c r="G762"/>
     </row>
-    <row r="763" spans="1:7">
+    <row r="763" spans="1:7" hidden="1">
       <c r="A763" t="s">
         <v>14</v>
       </c>
@@ -30885,7 +31028,7 @@
       </c>
       <c r="G763"/>
     </row>
-    <row r="764" spans="1:7">
+    <row r="764" spans="1:7" hidden="1">
       <c r="A764" t="s">
         <v>15</v>
       </c>
@@ -30906,7 +31049,7 @@
       </c>
       <c r="G764"/>
     </row>
-    <row r="765" spans="1:7">
+    <row r="765" spans="1:7" hidden="1">
       <c r="A765" t="s">
         <v>16</v>
       </c>
@@ -30927,7 +31070,7 @@
       </c>
       <c r="G765"/>
     </row>
-    <row r="766" spans="1:7">
+    <row r="766" spans="1:7" hidden="1">
       <c r="A766" t="s">
         <v>17</v>
       </c>
@@ -31893,7 +32036,7 @@
       </c>
       <c r="G811"/>
     </row>
-    <row r="812" spans="1:7">
+    <row r="812" spans="1:7" hidden="1">
       <c r="A812" t="s">
         <v>6</v>
       </c>
@@ -31914,7 +32057,7 @@
       </c>
       <c r="G812"/>
     </row>
-    <row r="813" spans="1:7">
+    <row r="813" spans="1:7" hidden="1">
       <c r="A813" t="s">
         <v>10</v>
       </c>
@@ -31935,7 +32078,7 @@
       </c>
       <c r="G813"/>
     </row>
-    <row r="814" spans="1:7">
+    <row r="814" spans="1:7" hidden="1">
       <c r="A814" t="s">
         <v>11</v>
       </c>
@@ -31956,7 +32099,7 @@
       </c>
       <c r="G814"/>
     </row>
-    <row r="815" spans="1:7">
+    <row r="815" spans="1:7" hidden="1">
       <c r="A815" t="s">
         <v>12</v>
       </c>
@@ -31977,7 +32120,7 @@
       </c>
       <c r="G815"/>
     </row>
-    <row r="816" spans="1:7">
+    <row r="816" spans="1:7" hidden="1">
       <c r="A816" t="s">
         <v>13</v>
       </c>
@@ -31998,7 +32141,7 @@
       </c>
       <c r="G816"/>
     </row>
-    <row r="817" spans="1:7">
+    <row r="817" spans="1:7" hidden="1">
       <c r="A817" t="s">
         <v>14</v>
       </c>
@@ -32019,7 +32162,7 @@
       </c>
       <c r="G817"/>
     </row>
-    <row r="818" spans="1:7">
+    <row r="818" spans="1:7" hidden="1">
       <c r="A818" t="s">
         <v>15</v>
       </c>
@@ -32040,7 +32183,7 @@
       </c>
       <c r="G818"/>
     </row>
-    <row r="819" spans="1:7">
+    <row r="819" spans="1:7" hidden="1">
       <c r="A819" t="s">
         <v>16</v>
       </c>
@@ -32061,7 +32204,7 @@
       </c>
       <c r="G819"/>
     </row>
-    <row r="820" spans="1:7">
+    <row r="820" spans="1:7" hidden="1">
       <c r="A820" t="s">
         <v>17</v>
       </c>
@@ -32460,7 +32603,7 @@
       </c>
       <c r="G838"/>
     </row>
-    <row r="839" spans="1:7">
+    <row r="839" spans="1:7" hidden="1">
       <c r="A839" t="s">
         <v>6</v>
       </c>
@@ -32481,7 +32624,7 @@
       </c>
       <c r="G839"/>
     </row>
-    <row r="840" spans="1:7">
+    <row r="840" spans="1:7" hidden="1">
       <c r="A840" t="s">
         <v>10</v>
       </c>
@@ -32502,7 +32645,7 @@
       </c>
       <c r="G840"/>
     </row>
-    <row r="841" spans="1:7">
+    <row r="841" spans="1:7" hidden="1">
       <c r="A841" t="s">
         <v>11</v>
       </c>
@@ -32523,7 +32666,7 @@
       </c>
       <c r="G841"/>
     </row>
-    <row r="842" spans="1:7">
+    <row r="842" spans="1:7" hidden="1">
       <c r="A842" t="s">
         <v>12</v>
       </c>
@@ -32544,7 +32687,7 @@
       </c>
       <c r="G842"/>
     </row>
-    <row r="843" spans="1:7">
+    <row r="843" spans="1:7" hidden="1">
       <c r="A843" t="s">
         <v>13</v>
       </c>
@@ -32565,7 +32708,7 @@
       </c>
       <c r="G843"/>
     </row>
-    <row r="844" spans="1:7">
+    <row r="844" spans="1:7" hidden="1">
       <c r="A844" t="s">
         <v>14</v>
       </c>
@@ -32586,7 +32729,7 @@
       </c>
       <c r="G844"/>
     </row>
-    <row r="845" spans="1:7">
+    <row r="845" spans="1:7" hidden="1">
       <c r="A845" t="s">
         <v>15</v>
       </c>
@@ -32607,7 +32750,7 @@
       </c>
       <c r="G845"/>
     </row>
-    <row r="846" spans="1:7">
+    <row r="846" spans="1:7" hidden="1">
       <c r="A846" t="s">
         <v>16</v>
       </c>
@@ -32628,7 +32771,7 @@
       </c>
       <c r="G846"/>
     </row>
-    <row r="847" spans="1:7">
+    <row r="847" spans="1:7" hidden="1">
       <c r="A847" t="s">
         <v>17</v>
       </c>
@@ -44577,7 +44720,7 @@
       </c>
       <c r="G1415"/>
     </row>
-    <row r="1416" spans="1:7" hidden="1">
+    <row r="1416" spans="1:7">
       <c r="A1416" t="s">
         <v>6</v>
       </c>
@@ -44598,7 +44741,7 @@
       </c>
       <c r="G1416"/>
     </row>
-    <row r="1417" spans="1:7" hidden="1">
+    <row r="1417" spans="1:7">
       <c r="A1417" t="s">
         <v>6</v>
       </c>
@@ -44619,7 +44762,7 @@
       </c>
       <c r="G1417"/>
     </row>
-    <row r="1418" spans="1:7" hidden="1">
+    <row r="1418" spans="1:7">
       <c r="A1418" t="s">
         <v>10</v>
       </c>
@@ -44640,7 +44783,7 @@
       </c>
       <c r="G1418"/>
     </row>
-    <row r="1419" spans="1:7" hidden="1">
+    <row r="1419" spans="1:7">
       <c r="A1419" t="s">
         <v>10</v>
       </c>
@@ -44661,7 +44804,7 @@
       </c>
       <c r="G1419"/>
     </row>
-    <row r="1420" spans="1:7" hidden="1">
+    <row r="1420" spans="1:7">
       <c r="A1420" t="s">
         <v>11</v>
       </c>
@@ -44682,7 +44825,7 @@
       </c>
       <c r="G1420"/>
     </row>
-    <row r="1421" spans="1:7" hidden="1">
+    <row r="1421" spans="1:7">
       <c r="A1421" t="s">
         <v>11</v>
       </c>
@@ -44703,7 +44846,7 @@
       </c>
       <c r="G1421"/>
     </row>
-    <row r="1422" spans="1:7" hidden="1">
+    <row r="1422" spans="1:7">
       <c r="A1422" t="s">
         <v>13</v>
       </c>
@@ -44724,7 +44867,7 @@
       </c>
       <c r="G1422"/>
     </row>
-    <row r="1423" spans="1:7" hidden="1">
+    <row r="1423" spans="1:7">
       <c r="A1423" t="s">
         <v>13</v>
       </c>
@@ -44745,7 +44888,7 @@
       </c>
       <c r="G1423"/>
     </row>
-    <row r="1424" spans="1:7" hidden="1">
+    <row r="1424" spans="1:7">
       <c r="A1424" t="s">
         <v>14</v>
       </c>
@@ -44766,7 +44909,7 @@
       </c>
       <c r="G1424"/>
     </row>
-    <row r="1425" spans="1:7" hidden="1">
+    <row r="1425" spans="1:7">
       <c r="A1425" t="s">
         <v>14</v>
       </c>
@@ -44787,7 +44930,7 @@
       </c>
       <c r="G1425"/>
     </row>
-    <row r="1426" spans="1:7" hidden="1">
+    <row r="1426" spans="1:7">
       <c r="A1426" t="s">
         <v>12</v>
       </c>
@@ -44808,7 +44951,7 @@
       </c>
       <c r="G1426"/>
     </row>
-    <row r="1427" spans="1:7" hidden="1">
+    <row r="1427" spans="1:7">
       <c r="A1427" t="s">
         <v>12</v>
       </c>
@@ -44829,7 +44972,7 @@
       </c>
       <c r="G1427"/>
     </row>
-    <row r="1428" spans="1:7" hidden="1">
+    <row r="1428" spans="1:7">
       <c r="A1428" t="s">
         <v>15</v>
       </c>
@@ -44850,7 +44993,7 @@
       </c>
       <c r="G1428"/>
     </row>
-    <row r="1429" spans="1:7" hidden="1">
+    <row r="1429" spans="1:7">
       <c r="A1429" t="s">
         <v>15</v>
       </c>
@@ -44871,7 +45014,7 @@
       </c>
       <c r="G1429"/>
     </row>
-    <row r="1430" spans="1:7" hidden="1">
+    <row r="1430" spans="1:7">
       <c r="A1430" t="s">
         <v>16</v>
       </c>
@@ -44892,7 +45035,7 @@
       </c>
       <c r="G1430"/>
     </row>
-    <row r="1431" spans="1:7" hidden="1">
+    <row r="1431" spans="1:7">
       <c r="A1431" t="s">
         <v>16</v>
       </c>
@@ -44913,7 +45056,7 @@
       </c>
       <c r="G1431"/>
     </row>
-    <row r="1432" spans="1:7" hidden="1">
+    <row r="1432" spans="1:7">
       <c r="A1432" t="s">
         <v>17</v>
       </c>
@@ -44934,7 +45077,7 @@
       </c>
       <c r="G1432"/>
     </row>
-    <row r="1433" spans="1:7" hidden="1">
+    <row r="1433" spans="1:7">
       <c r="A1433" t="s">
         <v>17</v>
       </c>
@@ -44955,7 +45098,7 @@
       </c>
       <c r="G1433"/>
     </row>
-    <row r="1434" spans="1:7">
+    <row r="1434" spans="1:7" hidden="1">
       <c r="A1434" s="5" t="s">
         <v>6</v>
       </c>
@@ -44976,7 +45119,7 @@
       </c>
       <c r="G1434"/>
     </row>
-    <row r="1435" spans="1:7">
+    <row r="1435" spans="1:7" hidden="1">
       <c r="A1435" s="5" t="s">
         <v>6</v>
       </c>
@@ -44997,7 +45140,7 @@
       </c>
       <c r="G1435"/>
     </row>
-    <row r="1436" spans="1:7">
+    <row r="1436" spans="1:7" hidden="1">
       <c r="A1436" s="5" t="s">
         <v>10</v>
       </c>
@@ -45018,7 +45161,7 @@
       </c>
       <c r="G1436"/>
     </row>
-    <row r="1437" spans="1:7">
+    <row r="1437" spans="1:7" hidden="1">
       <c r="A1437" s="5" t="s">
         <v>10</v>
       </c>
@@ -45039,7 +45182,7 @@
       </c>
       <c r="G1437"/>
     </row>
-    <row r="1438" spans="1:7">
+    <row r="1438" spans="1:7" hidden="1">
       <c r="A1438" s="5" t="s">
         <v>11</v>
       </c>
@@ -45060,7 +45203,7 @@
       </c>
       <c r="G1438"/>
     </row>
-    <row r="1439" spans="1:7">
+    <row r="1439" spans="1:7" hidden="1">
       <c r="A1439" s="5" t="s">
         <v>11</v>
       </c>
@@ -45081,7 +45224,7 @@
       </c>
       <c r="G1439"/>
     </row>
-    <row r="1440" spans="1:7">
+    <row r="1440" spans="1:7" hidden="1">
       <c r="A1440" s="5" t="s">
         <v>12</v>
       </c>
@@ -45102,7 +45245,7 @@
       </c>
       <c r="G1440"/>
     </row>
-    <row r="1441" spans="1:7">
+    <row r="1441" spans="1:7" hidden="1">
       <c r="A1441" s="5" t="s">
         <v>12</v>
       </c>
@@ -45123,7 +45266,7 @@
       </c>
       <c r="G1441"/>
     </row>
-    <row r="1442" spans="1:7">
+    <row r="1442" spans="1:7" hidden="1">
       <c r="A1442" s="5" t="s">
         <v>13</v>
       </c>
@@ -45144,7 +45287,7 @@
       </c>
       <c r="G1442"/>
     </row>
-    <row r="1443" spans="1:7">
+    <row r="1443" spans="1:7" hidden="1">
       <c r="A1443" s="5" t="s">
         <v>13</v>
       </c>
@@ -45165,7 +45308,7 @@
       </c>
       <c r="G1443"/>
     </row>
-    <row r="1444" spans="1:7">
+    <row r="1444" spans="1:7" hidden="1">
       <c r="A1444" s="5" t="s">
         <v>14</v>
       </c>
@@ -45186,7 +45329,7 @@
       </c>
       <c r="G1444"/>
     </row>
-    <row r="1445" spans="1:7">
+    <row r="1445" spans="1:7" hidden="1">
       <c r="A1445" s="5" t="s">
         <v>14</v>
       </c>
@@ -45207,7 +45350,7 @@
       </c>
       <c r="G1445"/>
     </row>
-    <row r="1446" spans="1:7">
+    <row r="1446" spans="1:7" hidden="1">
       <c r="A1446" s="5" t="s">
         <v>15</v>
       </c>
@@ -45228,7 +45371,7 @@
       </c>
       <c r="G1446"/>
     </row>
-    <row r="1447" spans="1:7">
+    <row r="1447" spans="1:7" hidden="1">
       <c r="A1447" s="5" t="s">
         <v>15</v>
       </c>
@@ -45249,7 +45392,7 @@
       </c>
       <c r="G1447"/>
     </row>
-    <row r="1448" spans="1:7">
+    <row r="1448" spans="1:7" hidden="1">
       <c r="A1448" s="5" t="s">
         <v>16</v>
       </c>
@@ -45270,7 +45413,7 @@
       </c>
       <c r="G1448"/>
     </row>
-    <row r="1449" spans="1:7">
+    <row r="1449" spans="1:7" hidden="1">
       <c r="A1449" s="5" t="s">
         <v>16</v>
       </c>
@@ -45291,7 +45434,7 @@
       </c>
       <c r="G1449"/>
     </row>
-    <row r="1450" spans="1:7">
+    <row r="1450" spans="1:7" hidden="1">
       <c r="A1450" s="5" t="s">
         <v>17</v>
       </c>
@@ -45312,7 +45455,7 @@
       </c>
       <c r="G1450"/>
     </row>
-    <row r="1451" spans="1:7">
+    <row r="1451" spans="1:7" hidden="1">
       <c r="A1451" s="5" t="s">
         <v>17</v>
       </c>
@@ -45715,14 +45858,7 @@
   <autoFilter ref="B1:B1469" xr:uid="{A58F1B57-0ED0-3247-9112-85DD1F029275}">
     <filterColumn colId="0">
       <filters>
-        <filter val="T_HDV_BS_CNG_R"/>
-        <filter val="T_HDV_BT_CNG_R"/>
-        <filter val="T_HDV_TCCNG_R"/>
-        <filter val="T_LDV_CCNG_R"/>
-        <filter val="T_LDV_FCNG_R"/>
-        <filter val="T_LDV_MVCNG_R"/>
-        <filter val="T_LDV_PCNG_R"/>
-        <filter val="T_MDV_TMCNG_R"/>
+        <filter val="T_HDV_THLDSL_R"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -45732,10 +45868,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E45044-B387-C440-9E53-EFE5C4A0945F}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -48206,7 +48342,1520 @@
       </c>
       <c r="J82" s="2"/>
     </row>
+    <row r="83" spans="1:10">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83" t="s">
+        <v>198</v>
+      </c>
+      <c r="D83" t="s">
+        <v>102</v>
+      </c>
+      <c r="E83">
+        <v>2018</v>
+      </c>
+      <c r="F83" t="s">
+        <v>199</v>
+      </c>
+      <c r="G83">
+        <v>15.32</v>
+      </c>
+      <c r="H83" t="s">
+        <v>87</v>
+      </c>
+      <c r="I83" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" t="s">
+        <v>198</v>
+      </c>
+      <c r="D84" t="s">
+        <v>102</v>
+      </c>
+      <c r="E84">
+        <v>2015</v>
+      </c>
+      <c r="F84" t="s">
+        <v>199</v>
+      </c>
+      <c r="G84">
+        <v>15.32</v>
+      </c>
+      <c r="H84" t="s">
+        <v>87</v>
+      </c>
+      <c r="I84" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" t="s">
+        <v>198</v>
+      </c>
+      <c r="D85" t="s">
+        <v>102</v>
+      </c>
+      <c r="E85">
+        <v>2018</v>
+      </c>
+      <c r="F85" t="s">
+        <v>199</v>
+      </c>
+      <c r="G85">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" t="s">
+        <v>198</v>
+      </c>
+      <c r="D86" t="s">
+        <v>102</v>
+      </c>
+      <c r="E86">
+        <v>2015</v>
+      </c>
+      <c r="F86" t="s">
+        <v>199</v>
+      </c>
+      <c r="G86">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H86" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>90</v>
+      </c>
+      <c r="C87" t="s">
+        <v>198</v>
+      </c>
+      <c r="D87" t="s">
+        <v>102</v>
+      </c>
+      <c r="E87">
+        <v>2018</v>
+      </c>
+      <c r="F87" t="s">
+        <v>199</v>
+      </c>
+      <c r="G87">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H87" t="s">
+        <v>87</v>
+      </c>
+      <c r="I87" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+      <c r="C88" t="s">
+        <v>198</v>
+      </c>
+      <c r="D88" t="s">
+        <v>102</v>
+      </c>
+      <c r="E88">
+        <v>2015</v>
+      </c>
+      <c r="F88" t="s">
+        <v>199</v>
+      </c>
+      <c r="G88">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H88" t="s">
+        <v>87</v>
+      </c>
+      <c r="I88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" t="s">
+        <v>86</v>
+      </c>
+      <c r="C89" t="s">
+        <v>198</v>
+      </c>
+      <c r="D89" t="s">
+        <v>102</v>
+      </c>
+      <c r="E89">
+        <v>2018</v>
+      </c>
+      <c r="F89" t="s">
+        <v>199</v>
+      </c>
+      <c r="G89">
+        <v>15.32</v>
+      </c>
+      <c r="H89" t="s">
+        <v>87</v>
+      </c>
+      <c r="I89" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" t="s">
+        <v>86</v>
+      </c>
+      <c r="C90" t="s">
+        <v>198</v>
+      </c>
+      <c r="D90" t="s">
+        <v>102</v>
+      </c>
+      <c r="E90">
+        <v>2015</v>
+      </c>
+      <c r="F90" t="s">
+        <v>199</v>
+      </c>
+      <c r="G90">
+        <v>15.32</v>
+      </c>
+      <c r="H90" t="s">
+        <v>87</v>
+      </c>
+      <c r="I90" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" t="s">
+        <v>89</v>
+      </c>
+      <c r="C91" t="s">
+        <v>198</v>
+      </c>
+      <c r="D91" t="s">
+        <v>102</v>
+      </c>
+      <c r="E91">
+        <v>2018</v>
+      </c>
+      <c r="F91" t="s">
+        <v>199</v>
+      </c>
+      <c r="G91">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H91" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" t="s">
+        <v>198</v>
+      </c>
+      <c r="D92" t="s">
+        <v>102</v>
+      </c>
+      <c r="E92">
+        <v>2015</v>
+      </c>
+      <c r="F92" t="s">
+        <v>199</v>
+      </c>
+      <c r="G92">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H92" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D93" t="s">
+        <v>102</v>
+      </c>
+      <c r="E93">
+        <v>2018</v>
+      </c>
+      <c r="F93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G93">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H93" t="s">
+        <v>87</v>
+      </c>
+      <c r="I93" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" t="s">
+        <v>90</v>
+      </c>
+      <c r="C94" t="s">
+        <v>198</v>
+      </c>
+      <c r="D94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E94">
+        <v>2015</v>
+      </c>
+      <c r="F94" t="s">
+        <v>199</v>
+      </c>
+      <c r="G94">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H94" t="s">
+        <v>87</v>
+      </c>
+      <c r="I94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" t="s">
+        <v>11</v>
+      </c>
+      <c r="B95" t="s">
+        <v>86</v>
+      </c>
+      <c r="C95" t="s">
+        <v>198</v>
+      </c>
+      <c r="D95" t="s">
+        <v>102</v>
+      </c>
+      <c r="E95">
+        <v>2018</v>
+      </c>
+      <c r="F95" t="s">
+        <v>199</v>
+      </c>
+      <c r="G95">
+        <v>15.32</v>
+      </c>
+      <c r="H95" t="s">
+        <v>87</v>
+      </c>
+      <c r="I95" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" t="s">
+        <v>86</v>
+      </c>
+      <c r="C96" t="s">
+        <v>198</v>
+      </c>
+      <c r="D96" t="s">
+        <v>102</v>
+      </c>
+      <c r="E96">
+        <v>2015</v>
+      </c>
+      <c r="F96" t="s">
+        <v>199</v>
+      </c>
+      <c r="G96">
+        <v>15.32</v>
+      </c>
+      <c r="H96" t="s">
+        <v>87</v>
+      </c>
+      <c r="I96" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" t="s">
+        <v>89</v>
+      </c>
+      <c r="C97" t="s">
+        <v>198</v>
+      </c>
+      <c r="D97" t="s">
+        <v>102</v>
+      </c>
+      <c r="E97">
+        <v>2018</v>
+      </c>
+      <c r="F97" t="s">
+        <v>199</v>
+      </c>
+      <c r="G97">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H97" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" t="s">
+        <v>89</v>
+      </c>
+      <c r="C98" t="s">
+        <v>198</v>
+      </c>
+      <c r="D98" t="s">
+        <v>102</v>
+      </c>
+      <c r="E98">
+        <v>2015</v>
+      </c>
+      <c r="F98" t="s">
+        <v>199</v>
+      </c>
+      <c r="G98">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" t="s">
+        <v>90</v>
+      </c>
+      <c r="C99" t="s">
+        <v>198</v>
+      </c>
+      <c r="D99" t="s">
+        <v>102</v>
+      </c>
+      <c r="E99">
+        <v>2018</v>
+      </c>
+      <c r="F99" t="s">
+        <v>199</v>
+      </c>
+      <c r="G99">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H99" t="s">
+        <v>87</v>
+      </c>
+      <c r="I99" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" t="s">
+        <v>90</v>
+      </c>
+      <c r="C100" t="s">
+        <v>198</v>
+      </c>
+      <c r="D100" t="s">
+        <v>102</v>
+      </c>
+      <c r="E100">
+        <v>2015</v>
+      </c>
+      <c r="F100" t="s">
+        <v>199</v>
+      </c>
+      <c r="G100">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H100" t="s">
+        <v>87</v>
+      </c>
+      <c r="I100" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>13</v>
+      </c>
+      <c r="B101" t="s">
+        <v>86</v>
+      </c>
+      <c r="C101" t="s">
+        <v>198</v>
+      </c>
+      <c r="D101" t="s">
+        <v>102</v>
+      </c>
+      <c r="E101">
+        <v>2018</v>
+      </c>
+      <c r="F101" t="s">
+        <v>199</v>
+      </c>
+      <c r="G101">
+        <v>15.32</v>
+      </c>
+      <c r="H101" t="s">
+        <v>87</v>
+      </c>
+      <c r="I101" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>13</v>
+      </c>
+      <c r="B102" t="s">
+        <v>86</v>
+      </c>
+      <c r="C102" t="s">
+        <v>198</v>
+      </c>
+      <c r="D102" t="s">
+        <v>102</v>
+      </c>
+      <c r="E102">
+        <v>2015</v>
+      </c>
+      <c r="F102" t="s">
+        <v>199</v>
+      </c>
+      <c r="G102">
+        <v>15.32</v>
+      </c>
+      <c r="H102" t="s">
+        <v>87</v>
+      </c>
+      <c r="I102" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>13</v>
+      </c>
+      <c r="B103" t="s">
+        <v>89</v>
+      </c>
+      <c r="C103" t="s">
+        <v>198</v>
+      </c>
+      <c r="D103" t="s">
+        <v>102</v>
+      </c>
+      <c r="E103">
+        <v>2018</v>
+      </c>
+      <c r="F103" t="s">
+        <v>199</v>
+      </c>
+      <c r="G103">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H103" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" t="s">
+        <v>89</v>
+      </c>
+      <c r="C104" t="s">
+        <v>198</v>
+      </c>
+      <c r="D104" t="s">
+        <v>102</v>
+      </c>
+      <c r="E104">
+        <v>2015</v>
+      </c>
+      <c r="F104" t="s">
+        <v>199</v>
+      </c>
+      <c r="G104">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H104" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>13</v>
+      </c>
+      <c r="B105" t="s">
+        <v>90</v>
+      </c>
+      <c r="C105" t="s">
+        <v>198</v>
+      </c>
+      <c r="D105" t="s">
+        <v>102</v>
+      </c>
+      <c r="E105">
+        <v>2018</v>
+      </c>
+      <c r="F105" t="s">
+        <v>199</v>
+      </c>
+      <c r="G105">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H105" t="s">
+        <v>87</v>
+      </c>
+      <c r="I105" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" t="s">
+        <v>90</v>
+      </c>
+      <c r="C106" t="s">
+        <v>198</v>
+      </c>
+      <c r="D106" t="s">
+        <v>102</v>
+      </c>
+      <c r="E106">
+        <v>2015</v>
+      </c>
+      <c r="F106" t="s">
+        <v>199</v>
+      </c>
+      <c r="G106">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H106" t="s">
+        <v>87</v>
+      </c>
+      <c r="I106" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" t="s">
+        <v>198</v>
+      </c>
+      <c r="D107" t="s">
+        <v>102</v>
+      </c>
+      <c r="E107">
+        <v>2018</v>
+      </c>
+      <c r="F107" t="s">
+        <v>199</v>
+      </c>
+      <c r="G107">
+        <v>15.32</v>
+      </c>
+      <c r="H107" t="s">
+        <v>87</v>
+      </c>
+      <c r="I107" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
+        <v>86</v>
+      </c>
+      <c r="C108" t="s">
+        <v>198</v>
+      </c>
+      <c r="D108" t="s">
+        <v>102</v>
+      </c>
+      <c r="E108">
+        <v>2015</v>
+      </c>
+      <c r="F108" t="s">
+        <v>199</v>
+      </c>
+      <c r="G108">
+        <v>15.32</v>
+      </c>
+      <c r="H108" t="s">
+        <v>87</v>
+      </c>
+      <c r="I108" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109" t="s">
+        <v>89</v>
+      </c>
+      <c r="C109" t="s">
+        <v>198</v>
+      </c>
+      <c r="D109" t="s">
+        <v>102</v>
+      </c>
+      <c r="E109">
+        <v>2018</v>
+      </c>
+      <c r="F109" t="s">
+        <v>199</v>
+      </c>
+      <c r="G109">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H109" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" t="s">
+        <v>89</v>
+      </c>
+      <c r="C110" t="s">
+        <v>198</v>
+      </c>
+      <c r="D110" t="s">
+        <v>102</v>
+      </c>
+      <c r="E110">
+        <v>2015</v>
+      </c>
+      <c r="F110" t="s">
+        <v>199</v>
+      </c>
+      <c r="G110">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H110" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>14</v>
+      </c>
+      <c r="B111" t="s">
+        <v>90</v>
+      </c>
+      <c r="C111" t="s">
+        <v>198</v>
+      </c>
+      <c r="D111" t="s">
+        <v>102</v>
+      </c>
+      <c r="E111">
+        <v>2018</v>
+      </c>
+      <c r="F111" t="s">
+        <v>199</v>
+      </c>
+      <c r="G111">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H111" t="s">
+        <v>87</v>
+      </c>
+      <c r="I111" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112" t="s">
+        <v>90</v>
+      </c>
+      <c r="C112" t="s">
+        <v>198</v>
+      </c>
+      <c r="D112" t="s">
+        <v>102</v>
+      </c>
+      <c r="E112">
+        <v>2015</v>
+      </c>
+      <c r="F112" t="s">
+        <v>199</v>
+      </c>
+      <c r="G112">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H112" t="s">
+        <v>87</v>
+      </c>
+      <c r="I112" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" t="s">
+        <v>86</v>
+      </c>
+      <c r="C113" t="s">
+        <v>198</v>
+      </c>
+      <c r="D113" t="s">
+        <v>102</v>
+      </c>
+      <c r="E113">
+        <v>2018</v>
+      </c>
+      <c r="F113" t="s">
+        <v>199</v>
+      </c>
+      <c r="G113">
+        <v>15.32</v>
+      </c>
+      <c r="H113" t="s">
+        <v>87</v>
+      </c>
+      <c r="I113" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" t="s">
+        <v>86</v>
+      </c>
+      <c r="C114" t="s">
+        <v>198</v>
+      </c>
+      <c r="D114" t="s">
+        <v>102</v>
+      </c>
+      <c r="E114">
+        <v>2015</v>
+      </c>
+      <c r="F114" t="s">
+        <v>199</v>
+      </c>
+      <c r="G114">
+        <v>15.32</v>
+      </c>
+      <c r="H114" t="s">
+        <v>87</v>
+      </c>
+      <c r="I114" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>12</v>
+      </c>
+      <c r="B115" t="s">
+        <v>89</v>
+      </c>
+      <c r="C115" t="s">
+        <v>198</v>
+      </c>
+      <c r="D115" t="s">
+        <v>102</v>
+      </c>
+      <c r="E115">
+        <v>2018</v>
+      </c>
+      <c r="F115" t="s">
+        <v>199</v>
+      </c>
+      <c r="G115">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H115" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116" t="s">
+        <v>89</v>
+      </c>
+      <c r="C116" t="s">
+        <v>198</v>
+      </c>
+      <c r="D116" t="s">
+        <v>102</v>
+      </c>
+      <c r="E116">
+        <v>2015</v>
+      </c>
+      <c r="F116" t="s">
+        <v>199</v>
+      </c>
+      <c r="G116">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H116" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" t="s">
+        <v>90</v>
+      </c>
+      <c r="C117" t="s">
+        <v>198</v>
+      </c>
+      <c r="D117" t="s">
+        <v>102</v>
+      </c>
+      <c r="E117">
+        <v>2018</v>
+      </c>
+      <c r="F117" t="s">
+        <v>199</v>
+      </c>
+      <c r="G117">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H117" t="s">
+        <v>87</v>
+      </c>
+      <c r="I117" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118" t="s">
+        <v>90</v>
+      </c>
+      <c r="C118" t="s">
+        <v>198</v>
+      </c>
+      <c r="D118" t="s">
+        <v>102</v>
+      </c>
+      <c r="E118">
+        <v>2015</v>
+      </c>
+      <c r="F118" t="s">
+        <v>199</v>
+      </c>
+      <c r="G118">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H118" t="s">
+        <v>87</v>
+      </c>
+      <c r="I118" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>15</v>
+      </c>
+      <c r="B119" t="s">
+        <v>86</v>
+      </c>
+      <c r="C119" t="s">
+        <v>198</v>
+      </c>
+      <c r="D119" t="s">
+        <v>102</v>
+      </c>
+      <c r="E119">
+        <v>2018</v>
+      </c>
+      <c r="F119" t="s">
+        <v>199</v>
+      </c>
+      <c r="G119">
+        <v>15.32</v>
+      </c>
+      <c r="H119" t="s">
+        <v>87</v>
+      </c>
+      <c r="I119" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>15</v>
+      </c>
+      <c r="B120" t="s">
+        <v>86</v>
+      </c>
+      <c r="C120" t="s">
+        <v>198</v>
+      </c>
+      <c r="D120" t="s">
+        <v>102</v>
+      </c>
+      <c r="E120">
+        <v>2015</v>
+      </c>
+      <c r="F120" t="s">
+        <v>199</v>
+      </c>
+      <c r="G120">
+        <v>15.32</v>
+      </c>
+      <c r="H120" t="s">
+        <v>87</v>
+      </c>
+      <c r="I120" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>15</v>
+      </c>
+      <c r="B121" t="s">
+        <v>89</v>
+      </c>
+      <c r="C121" t="s">
+        <v>198</v>
+      </c>
+      <c r="D121" t="s">
+        <v>102</v>
+      </c>
+      <c r="E121">
+        <v>2018</v>
+      </c>
+      <c r="F121" t="s">
+        <v>199</v>
+      </c>
+      <c r="G121">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H121" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>15</v>
+      </c>
+      <c r="B122" t="s">
+        <v>89</v>
+      </c>
+      <c r="C122" t="s">
+        <v>198</v>
+      </c>
+      <c r="D122" t="s">
+        <v>102</v>
+      </c>
+      <c r="E122">
+        <v>2015</v>
+      </c>
+      <c r="F122" t="s">
+        <v>199</v>
+      </c>
+      <c r="G122">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H122" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
+        <v>15</v>
+      </c>
+      <c r="B123" t="s">
+        <v>90</v>
+      </c>
+      <c r="C123" t="s">
+        <v>198</v>
+      </c>
+      <c r="D123" t="s">
+        <v>102</v>
+      </c>
+      <c r="E123">
+        <v>2018</v>
+      </c>
+      <c r="F123" t="s">
+        <v>199</v>
+      </c>
+      <c r="G123">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H123" t="s">
+        <v>87</v>
+      </c>
+      <c r="I123" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" t="s">
+        <v>15</v>
+      </c>
+      <c r="B124" t="s">
+        <v>90</v>
+      </c>
+      <c r="C124" t="s">
+        <v>198</v>
+      </c>
+      <c r="D124" t="s">
+        <v>102</v>
+      </c>
+      <c r="E124">
+        <v>2015</v>
+      </c>
+      <c r="F124" t="s">
+        <v>199</v>
+      </c>
+      <c r="G124">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H124" t="s">
+        <v>87</v>
+      </c>
+      <c r="I124" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" t="s">
+        <v>16</v>
+      </c>
+      <c r="B125" t="s">
+        <v>86</v>
+      </c>
+      <c r="C125" t="s">
+        <v>198</v>
+      </c>
+      <c r="D125" t="s">
+        <v>102</v>
+      </c>
+      <c r="E125">
+        <v>2018</v>
+      </c>
+      <c r="F125" t="s">
+        <v>199</v>
+      </c>
+      <c r="G125">
+        <v>15.32</v>
+      </c>
+      <c r="H125" t="s">
+        <v>87</v>
+      </c>
+      <c r="I125" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" t="s">
+        <v>16</v>
+      </c>
+      <c r="B126" t="s">
+        <v>86</v>
+      </c>
+      <c r="C126" t="s">
+        <v>198</v>
+      </c>
+      <c r="D126" t="s">
+        <v>102</v>
+      </c>
+      <c r="E126">
+        <v>2015</v>
+      </c>
+      <c r="F126" t="s">
+        <v>199</v>
+      </c>
+      <c r="G126">
+        <v>15.32</v>
+      </c>
+      <c r="H126" t="s">
+        <v>87</v>
+      </c>
+      <c r="I126" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" t="s">
+        <v>16</v>
+      </c>
+      <c r="B127" t="s">
+        <v>89</v>
+      </c>
+      <c r="C127" t="s">
+        <v>198</v>
+      </c>
+      <c r="D127" t="s">
+        <v>102</v>
+      </c>
+      <c r="E127">
+        <v>2018</v>
+      </c>
+      <c r="F127" t="s">
+        <v>199</v>
+      </c>
+      <c r="G127">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H127" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" t="s">
+        <v>16</v>
+      </c>
+      <c r="B128" t="s">
+        <v>89</v>
+      </c>
+      <c r="C128" t="s">
+        <v>198</v>
+      </c>
+      <c r="D128" t="s">
+        <v>102</v>
+      </c>
+      <c r="E128">
+        <v>2015</v>
+      </c>
+      <c r="F128" t="s">
+        <v>199</v>
+      </c>
+      <c r="G128">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H128" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129" t="s">
+        <v>16</v>
+      </c>
+      <c r="B129" t="s">
+        <v>90</v>
+      </c>
+      <c r="C129" t="s">
+        <v>198</v>
+      </c>
+      <c r="D129" t="s">
+        <v>102</v>
+      </c>
+      <c r="E129">
+        <v>2018</v>
+      </c>
+      <c r="F129" t="s">
+        <v>199</v>
+      </c>
+      <c r="G129">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H129" t="s">
+        <v>87</v>
+      </c>
+      <c r="I129" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130" t="s">
+        <v>16</v>
+      </c>
+      <c r="B130" t="s">
+        <v>90</v>
+      </c>
+      <c r="C130" t="s">
+        <v>198</v>
+      </c>
+      <c r="D130" t="s">
+        <v>102</v>
+      </c>
+      <c r="E130">
+        <v>2015</v>
+      </c>
+      <c r="F130" t="s">
+        <v>199</v>
+      </c>
+      <c r="G130">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H130" t="s">
+        <v>87</v>
+      </c>
+      <c r="I130" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" t="s">
+        <v>17</v>
+      </c>
+      <c r="B131" t="s">
+        <v>86</v>
+      </c>
+      <c r="C131" t="s">
+        <v>198</v>
+      </c>
+      <c r="D131" t="s">
+        <v>102</v>
+      </c>
+      <c r="E131">
+        <v>2018</v>
+      </c>
+      <c r="F131" t="s">
+        <v>199</v>
+      </c>
+      <c r="G131">
+        <v>15.32</v>
+      </c>
+      <c r="H131" t="s">
+        <v>87</v>
+      </c>
+      <c r="I131" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" t="s">
+        <v>17</v>
+      </c>
+      <c r="B132" t="s">
+        <v>86</v>
+      </c>
+      <c r="C132" t="s">
+        <v>198</v>
+      </c>
+      <c r="D132" t="s">
+        <v>102</v>
+      </c>
+      <c r="E132">
+        <v>2015</v>
+      </c>
+      <c r="F132" t="s">
+        <v>199</v>
+      </c>
+      <c r="G132">
+        <v>15.32</v>
+      </c>
+      <c r="H132" t="s">
+        <v>87</v>
+      </c>
+      <c r="I132" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" t="s">
+        <v>17</v>
+      </c>
+      <c r="B133" t="s">
+        <v>89</v>
+      </c>
+      <c r="C133" t="s">
+        <v>198</v>
+      </c>
+      <c r="D133" t="s">
+        <v>102</v>
+      </c>
+      <c r="E133">
+        <v>2018</v>
+      </c>
+      <c r="F133" t="s">
+        <v>199</v>
+      </c>
+      <c r="G133">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H133" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" t="s">
+        <v>17</v>
+      </c>
+      <c r="B134" t="s">
+        <v>89</v>
+      </c>
+      <c r="C134" t="s">
+        <v>198</v>
+      </c>
+      <c r="D134" t="s">
+        <v>102</v>
+      </c>
+      <c r="E134">
+        <v>2015</v>
+      </c>
+      <c r="F134" t="s">
+        <v>199</v>
+      </c>
+      <c r="G134">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H134" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135" t="s">
+        <v>17</v>
+      </c>
+      <c r="B135" t="s">
+        <v>90</v>
+      </c>
+      <c r="C135" t="s">
+        <v>198</v>
+      </c>
+      <c r="D135" t="s">
+        <v>102</v>
+      </c>
+      <c r="E135">
+        <v>2018</v>
+      </c>
+      <c r="F135" t="s">
+        <v>199</v>
+      </c>
+      <c r="G135">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H135" t="s">
+        <v>87</v>
+      </c>
+      <c r="I135" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" t="s">
+        <v>17</v>
+      </c>
+      <c r="B136" t="s">
+        <v>90</v>
+      </c>
+      <c r="C136" t="s">
+        <v>198</v>
+      </c>
+      <c r="D136" t="s">
+        <v>102</v>
+      </c>
+      <c r="E136">
+        <v>2015</v>
+      </c>
+      <c r="F136" t="s">
+        <v>199</v>
+      </c>
+      <c r="G136">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H136" t="s">
+        <v>87</v>
+      </c>
+      <c r="I136" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I136" xr:uid="{53A636C6-2F56-BB45-9E84-D95EC8C8B980}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -48443,10 +50092,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2737C6E4-DD82-2048-A722-D97786E2AA4E}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD19"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="Q89" sqref="Q89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -50341,6 +51990,420 @@
         <v>83</v>
       </c>
     </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>198</v>
+      </c>
+      <c r="C83" t="s">
+        <v>102</v>
+      </c>
+      <c r="D83">
+        <v>2018</v>
+      </c>
+      <c r="E83" t="s">
+        <v>199</v>
+      </c>
+      <c r="F83">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G83" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>198</v>
+      </c>
+      <c r="C84" t="s">
+        <v>102</v>
+      </c>
+      <c r="D84">
+        <v>2015</v>
+      </c>
+      <c r="E84" t="s">
+        <v>199</v>
+      </c>
+      <c r="F84">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G84" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" t="s">
+        <v>102</v>
+      </c>
+      <c r="D85">
+        <v>2018</v>
+      </c>
+      <c r="E85" t="s">
+        <v>199</v>
+      </c>
+      <c r="F85">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G85" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" t="s">
+        <v>198</v>
+      </c>
+      <c r="C86" t="s">
+        <v>102</v>
+      </c>
+      <c r="D86">
+        <v>2015</v>
+      </c>
+      <c r="E86" t="s">
+        <v>199</v>
+      </c>
+      <c r="F86">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G86" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" t="s">
+        <v>198</v>
+      </c>
+      <c r="C87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D87">
+        <v>2018</v>
+      </c>
+      <c r="E87" t="s">
+        <v>199</v>
+      </c>
+      <c r="F87">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G87" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" t="s">
+        <v>102</v>
+      </c>
+      <c r="D88">
+        <v>2015</v>
+      </c>
+      <c r="E88" t="s">
+        <v>199</v>
+      </c>
+      <c r="F88">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G88" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" t="s">
+        <v>198</v>
+      </c>
+      <c r="C89" t="s">
+        <v>102</v>
+      </c>
+      <c r="D89">
+        <v>2018</v>
+      </c>
+      <c r="E89" t="s">
+        <v>199</v>
+      </c>
+      <c r="F89">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G89" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" t="s">
+        <v>198</v>
+      </c>
+      <c r="C90" t="s">
+        <v>102</v>
+      </c>
+      <c r="D90">
+        <v>2015</v>
+      </c>
+      <c r="E90" t="s">
+        <v>199</v>
+      </c>
+      <c r="F90">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G90" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" t="s">
+        <v>198</v>
+      </c>
+      <c r="C91" t="s">
+        <v>102</v>
+      </c>
+      <c r="D91">
+        <v>2018</v>
+      </c>
+      <c r="E91" t="s">
+        <v>199</v>
+      </c>
+      <c r="F91">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G91" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" t="s">
+        <v>198</v>
+      </c>
+      <c r="C92" t="s">
+        <v>102</v>
+      </c>
+      <c r="D92">
+        <v>2015</v>
+      </c>
+      <c r="E92" t="s">
+        <v>199</v>
+      </c>
+      <c r="F92">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G92" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" t="s">
+        <v>198</v>
+      </c>
+      <c r="C93" t="s">
+        <v>102</v>
+      </c>
+      <c r="D93">
+        <v>2018</v>
+      </c>
+      <c r="E93" t="s">
+        <v>199</v>
+      </c>
+      <c r="F93">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G93" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" t="s">
+        <v>198</v>
+      </c>
+      <c r="C94" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94">
+        <v>2015</v>
+      </c>
+      <c r="E94" t="s">
+        <v>199</v>
+      </c>
+      <c r="F94">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G94" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>15</v>
+      </c>
+      <c r="B95" t="s">
+        <v>198</v>
+      </c>
+      <c r="C95" t="s">
+        <v>102</v>
+      </c>
+      <c r="D95">
+        <v>2018</v>
+      </c>
+      <c r="E95" t="s">
+        <v>199</v>
+      </c>
+      <c r="F95">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G95" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" t="s">
+        <v>198</v>
+      </c>
+      <c r="C96" t="s">
+        <v>102</v>
+      </c>
+      <c r="D96">
+        <v>2015</v>
+      </c>
+      <c r="E96" t="s">
+        <v>199</v>
+      </c>
+      <c r="F96">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G96" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B97" t="s">
+        <v>198</v>
+      </c>
+      <c r="C97" t="s">
+        <v>102</v>
+      </c>
+      <c r="D97">
+        <v>2018</v>
+      </c>
+      <c r="E97" t="s">
+        <v>199</v>
+      </c>
+      <c r="F97">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G97" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B98" t="s">
+        <v>198</v>
+      </c>
+      <c r="C98" t="s">
+        <v>102</v>
+      </c>
+      <c r="D98">
+        <v>2015</v>
+      </c>
+      <c r="E98" t="s">
+        <v>199</v>
+      </c>
+      <c r="F98">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G98" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99" t="s">
+        <v>198</v>
+      </c>
+      <c r="C99" t="s">
+        <v>102</v>
+      </c>
+      <c r="D99">
+        <v>2018</v>
+      </c>
+      <c r="E99" t="s">
+        <v>199</v>
+      </c>
+      <c r="F99">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G99" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100" t="s">
+        <v>198</v>
+      </c>
+      <c r="C100" t="s">
+        <v>102</v>
+      </c>
+      <c r="D100">
+        <v>2015</v>
+      </c>
+      <c r="E100" t="s">
+        <v>199</v>
+      </c>
+      <c r="F100">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G100" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G82" xr:uid="{2737C6E4-DD82-2048-A722-D97786E2AA4E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50348,10 +52411,465 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE438D4-1BF8-0947-90AC-2AC0B0A50AAD}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2">
+        <v>2018</v>
+      </c>
+      <c r="E2">
+        <v>152</v>
+      </c>
+      <c r="F2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
+        <v>2015</v>
+      </c>
+      <c r="E3">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
+        <v>2018</v>
+      </c>
+      <c r="E4">
+        <v>152</v>
+      </c>
+      <c r="F4" t="s">
+        <v>202</v>
+      </c>
+      <c r="G4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5">
+        <v>2015</v>
+      </c>
+      <c r="E5">
+        <v>152</v>
+      </c>
+      <c r="F5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6">
+        <v>2018</v>
+      </c>
+      <c r="E6">
+        <v>152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7">
+        <v>2015</v>
+      </c>
+      <c r="E7">
+        <v>152</v>
+      </c>
+      <c r="F7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2020</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8">
+        <v>2018</v>
+      </c>
+      <c r="E8">
+        <v>152</v>
+      </c>
+      <c r="F8" t="s">
+        <v>202</v>
+      </c>
+      <c r="G8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>2020</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9">
+        <v>2015</v>
+      </c>
+      <c r="E9">
+        <v>152</v>
+      </c>
+      <c r="F9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>2020</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10">
+        <v>2018</v>
+      </c>
+      <c r="E10">
+        <v>152</v>
+      </c>
+      <c r="F10" t="s">
+        <v>202</v>
+      </c>
+      <c r="G10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>2020</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11">
+        <v>2015</v>
+      </c>
+      <c r="E11">
+        <v>152</v>
+      </c>
+      <c r="F11" t="s">
+        <v>202</v>
+      </c>
+      <c r="G11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12">
+        <v>2018</v>
+      </c>
+      <c r="E12">
+        <v>152</v>
+      </c>
+      <c r="F12" t="s">
+        <v>202</v>
+      </c>
+      <c r="G12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2020</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13">
+        <v>2015</v>
+      </c>
+      <c r="E13">
+        <v>152</v>
+      </c>
+      <c r="F13" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>2020</v>
+      </c>
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14">
+        <v>2018</v>
+      </c>
+      <c r="E14">
+        <v>152</v>
+      </c>
+      <c r="F14" t="s">
+        <v>202</v>
+      </c>
+      <c r="G14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>2020</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15">
+        <v>2015</v>
+      </c>
+      <c r="E15">
+        <v>152</v>
+      </c>
+      <c r="F15" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>2020</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16">
+        <v>2018</v>
+      </c>
+      <c r="E16">
+        <v>152</v>
+      </c>
+      <c r="F16" t="s">
+        <v>202</v>
+      </c>
+      <c r="G16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2020</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17">
+        <v>2015</v>
+      </c>
+      <c r="E17">
+        <v>152</v>
+      </c>
+      <c r="F17" t="s">
+        <v>202</v>
+      </c>
+      <c r="G17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2020</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18">
+        <v>2018</v>
+      </c>
+      <c r="E18">
+        <v>152</v>
+      </c>
+      <c r="F18" t="s">
+        <v>202</v>
+      </c>
+      <c r="G18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>2020</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19">
+        <v>2015</v>
+      </c>
+      <c r="E19">
+        <v>152</v>
+      </c>
+      <c r="F19" t="s">
+        <v>202</v>
+      </c>
+      <c r="G19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98C7A7F-43E6-E642-9F02-ED0DAC40D0AF}">
   <dimension ref="A1:F1037"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
@@ -71107,7 +73625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DEA52A-DD20-5F43-9CC3-3845584BAF4F}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -71170,7 +73688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CED1427-52C6-644B-BCE1-B4BE9D18E414}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -71204,119 +73722,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E93042-7294-BF4C-AE0A-DBD708DEC29E}">
-  <dimension ref="A1:A20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add 2018 THLDSL vintage to transport_regionalization_master (#57)
</commit_message>
<xml_diff>
--- a/data_aggregation/transport/transport_regionalization_master.xlsx
+++ b/data_aggregation/transport/transport_regionalization_master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiejordan/Documents/GitHub/kathjordan_oeo/data_aggregation/transport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiejordan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7564BE12-A6E7-5649-9E85-3FF6FE13DFF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F28A2B7-E596-7649-80CA-FDBB822AE7CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30580" yWindow="-40" windowWidth="24500" windowHeight="16360" xr2:uid="{E784C07B-F067-AC4C-95FD-EC182FDC45A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22420" windowHeight="17500" activeTab="1" xr2:uid="{E784C07B-F067-AC4C-95FD-EC182FDC45A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand" sheetId="3" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="EmissionActivity" sheetId="7" r:id="rId3"/>
     <sheet name="LifetimeTech" sheetId="9" r:id="rId4"/>
     <sheet name="Efficiency" sheetId="2" r:id="rId5"/>
-    <sheet name="TechInputSplit" sheetId="4" r:id="rId6"/>
-    <sheet name="technologies" sheetId="5" r:id="rId7"/>
-    <sheet name="tech_annual" sheetId="6" r:id="rId8"/>
-    <sheet name="needs deleting" sheetId="8" r:id="rId9"/>
+    <sheet name="CostVariable" sheetId="10" r:id="rId6"/>
+    <sheet name="TechInputSplit" sheetId="4" r:id="rId7"/>
+    <sheet name="technologies" sheetId="5" r:id="rId8"/>
+    <sheet name="tech_annual" sheetId="6" r:id="rId9"/>
+    <sheet name="needs deleting" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Demand!$A$1:$F$743</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Efficiency!$A$1:$G$82</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EmissionActivity!$A$1:$I$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EmissionActivity!$A$1:$I$136</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ExistingCapacity!$B$1:$B$1469</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5" concurrentCalc="0"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13933" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14462" uniqueCount="207">
   <si>
     <t>regions</t>
   </si>
@@ -642,6 +643,33 @@
   <si>
     <t>ELC_TRN</t>
   </si>
+  <si>
+    <t>DSL</t>
+  </si>
+  <si>
+    <t>TMDHDV_HTL_DSL</t>
+  </si>
+  <si>
+    <t>#VT_EPAUS9rT_TRNHDV_v18.1.1full.xlsx, TechData_HDV_EMIS</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy21osti/71796.pdf figure 25</t>
+  </si>
+  <si>
+    <t>M$/bvmt</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy21osti/71796.pdf table 5</t>
+  </si>
+  <si>
+    <t>cost_variable</t>
+  </si>
+  <si>
+    <t>cost_variable_units</t>
+  </si>
+  <si>
+    <t>cost_variable_notes</t>
+  </si>
 </sst>
 </file>
 
@@ -1020,7 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5BAA25-0133-4242-BE9A-4343197BBF61}">
   <dimension ref="A1:F743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H161" sqref="H161"/>
     </sheetView>
   </sheetViews>
@@ -15710,13 +15738,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E93042-7294-BF4C-AE0A-DBD708DEC29E}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90557C9-C767-8C4E-81AD-DC2D04727A3B}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G1469"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E680" sqref="E680"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1418" sqref="D1418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15746,7 +15889,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" hidden="1">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -15872,7 +16015,7 @@
       </c>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" hidden="1">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -16081,7 +16224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:6" customFormat="1">
+    <row r="18" spans="1:6" customFormat="1" hidden="1">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -16181,7 +16324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" customFormat="1">
+    <row r="23" spans="1:6" customFormat="1" hidden="1">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -16361,7 +16504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:6" customFormat="1">
+    <row r="32" spans="1:6" customFormat="1" hidden="1">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -16481,7 +16624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" customFormat="1">
+    <row r="38" spans="1:6" customFormat="1" hidden="1">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -16681,7 +16824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:6" customFormat="1">
+    <row r="48" spans="1:6" customFormat="1" hidden="1">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -16781,7 +16924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:6" customFormat="1">
+    <row r="53" spans="1:6" customFormat="1" hidden="1">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -16961,7 +17104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:6" customFormat="1">
+    <row r="62" spans="1:6" customFormat="1" hidden="1">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -17081,7 +17224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:6" customFormat="1">
+    <row r="68" spans="1:6" customFormat="1" hidden="1">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -17281,7 +17424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="78" spans="1:6" customFormat="1">
+    <row r="78" spans="1:6" customFormat="1" hidden="1">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -17381,7 +17524,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:6" customFormat="1">
+    <row r="83" spans="1:6" customFormat="1" hidden="1">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -17561,7 +17704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:6" customFormat="1">
+    <row r="92" spans="1:6" customFormat="1" hidden="1">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -17681,7 +17824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="1:6" customFormat="1">
+    <row r="98" spans="1:6" customFormat="1" hidden="1">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -17881,7 +18024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="108" spans="1:6" customFormat="1">
+    <row r="108" spans="1:6" customFormat="1" hidden="1">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -17981,7 +18124,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:6" customFormat="1">
+    <row r="113" spans="1:6" customFormat="1" hidden="1">
       <c r="A113" t="s">
         <v>12</v>
       </c>
@@ -18161,7 +18304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="122" spans="1:6" customFormat="1">
+    <row r="122" spans="1:6" customFormat="1" hidden="1">
       <c r="A122" t="s">
         <v>13</v>
       </c>
@@ -18281,7 +18424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="1:6" customFormat="1">
+    <row r="128" spans="1:6" customFormat="1" hidden="1">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -18481,7 +18624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="138" spans="1:6" customFormat="1">
+    <row r="138" spans="1:6" customFormat="1" hidden="1">
       <c r="A138" t="s">
         <v>13</v>
       </c>
@@ -18581,7 +18724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="143" spans="1:6" customFormat="1">
+    <row r="143" spans="1:6" customFormat="1" hidden="1">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -18761,7 +18904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:6" customFormat="1">
+    <row r="152" spans="1:6" customFormat="1" hidden="1">
       <c r="A152" t="s">
         <v>14</v>
       </c>
@@ -18881,7 +19024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="158" spans="1:6" customFormat="1">
+    <row r="158" spans="1:6" customFormat="1" hidden="1">
       <c r="A158" t="s">
         <v>14</v>
       </c>
@@ -19081,7 +19224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:6" customFormat="1">
+    <row r="168" spans="1:6" customFormat="1" hidden="1">
       <c r="A168" t="s">
         <v>14</v>
       </c>
@@ -19181,7 +19324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:6" customFormat="1">
+    <row r="173" spans="1:6" customFormat="1" hidden="1">
       <c r="A173" t="s">
         <v>14</v>
       </c>
@@ -19361,7 +19504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:6" customFormat="1">
+    <row r="182" spans="1:6" customFormat="1" hidden="1">
       <c r="A182" t="s">
         <v>15</v>
       </c>
@@ -19481,7 +19624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:6" customFormat="1">
+    <row r="188" spans="1:6" customFormat="1" hidden="1">
       <c r="A188" t="s">
         <v>15</v>
       </c>
@@ -19681,7 +19824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:6" customFormat="1">
+    <row r="198" spans="1:6" customFormat="1" hidden="1">
       <c r="A198" t="s">
         <v>15</v>
       </c>
@@ -19781,7 +19924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:6" customFormat="1">
+    <row r="203" spans="1:6" customFormat="1" hidden="1">
       <c r="A203" t="s">
         <v>15</v>
       </c>
@@ -19961,7 +20104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="212" spans="1:6" customFormat="1">
+    <row r="212" spans="1:6" customFormat="1" hidden="1">
       <c r="A212" t="s">
         <v>16</v>
       </c>
@@ -20081,7 +20224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="218" spans="1:6" customFormat="1">
+    <row r="218" spans="1:6" customFormat="1" hidden="1">
       <c r="A218" t="s">
         <v>16</v>
       </c>
@@ -20281,7 +20424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="228" spans="1:6" customFormat="1">
+    <row r="228" spans="1:6" customFormat="1" hidden="1">
       <c r="A228" t="s">
         <v>16</v>
       </c>
@@ -20381,7 +20524,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:6" customFormat="1">
+    <row r="233" spans="1:6" customFormat="1" hidden="1">
       <c r="A233" t="s">
         <v>16</v>
       </c>
@@ -20561,7 +20704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="242" spans="1:6" customFormat="1">
+    <row r="242" spans="1:6" customFormat="1" hidden="1">
       <c r="A242" t="s">
         <v>17</v>
       </c>
@@ -20681,7 +20824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="248" spans="1:6" customFormat="1">
+    <row r="248" spans="1:6" customFormat="1" hidden="1">
       <c r="A248" t="s">
         <v>17</v>
       </c>
@@ -20881,7 +21024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="258" spans="1:6" customFormat="1">
+    <row r="258" spans="1:6" customFormat="1" hidden="1">
       <c r="A258" t="s">
         <v>17</v>
       </c>
@@ -20981,7 +21124,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="263" spans="1:6" customFormat="1">
+    <row r="263" spans="1:6" customFormat="1" hidden="1">
       <c r="A263" t="s">
         <v>17</v>
       </c>
@@ -21161,7 +21304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="272" spans="1:6" customFormat="1">
+    <row r="272" spans="1:6" customFormat="1" hidden="1">
       <c r="A272" t="s">
         <v>6</v>
       </c>
@@ -21281,7 +21424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="278" spans="1:6" customFormat="1">
+    <row r="278" spans="1:6" customFormat="1" hidden="1">
       <c r="A278" t="s">
         <v>6</v>
       </c>
@@ -21481,7 +21624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="288" spans="1:6" customFormat="1">
+    <row r="288" spans="1:6" customFormat="1" hidden="1">
       <c r="A288" t="s">
         <v>6</v>
       </c>
@@ -21581,7 +21724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="293" spans="1:6" customFormat="1">
+    <row r="293" spans="1:6" customFormat="1" hidden="1">
       <c r="A293" t="s">
         <v>6</v>
       </c>
@@ -21761,7 +21904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="302" spans="1:6" customFormat="1">
+    <row r="302" spans="1:6" customFormat="1" hidden="1">
       <c r="A302" t="s">
         <v>10</v>
       </c>
@@ -21881,7 +22024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="308" spans="1:6" customFormat="1">
+    <row r="308" spans="1:6" customFormat="1" hidden="1">
       <c r="A308" t="s">
         <v>10</v>
       </c>
@@ -22081,7 +22224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="318" spans="1:6" customFormat="1">
+    <row r="318" spans="1:6" customFormat="1" hidden="1">
       <c r="A318" t="s">
         <v>10</v>
       </c>
@@ -22181,7 +22324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="323" spans="1:6" customFormat="1">
+    <row r="323" spans="1:6" customFormat="1" hidden="1">
       <c r="A323" t="s">
         <v>10</v>
       </c>
@@ -22361,7 +22504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="332" spans="1:6" customFormat="1">
+    <row r="332" spans="1:6" customFormat="1" hidden="1">
       <c r="A332" t="s">
         <v>11</v>
       </c>
@@ -22481,7 +22624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="338" spans="1:6" customFormat="1">
+    <row r="338" spans="1:6" customFormat="1" hidden="1">
       <c r="A338" t="s">
         <v>11</v>
       </c>
@@ -22681,7 +22824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="348" spans="1:6" customFormat="1">
+    <row r="348" spans="1:6" customFormat="1" hidden="1">
       <c r="A348" t="s">
         <v>11</v>
       </c>
@@ -22781,7 +22924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="353" spans="1:6" customFormat="1">
+    <row r="353" spans="1:6" customFormat="1" hidden="1">
       <c r="A353" t="s">
         <v>11</v>
       </c>
@@ -22961,7 +23104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="362" spans="1:6" customFormat="1">
+    <row r="362" spans="1:6" customFormat="1" hidden="1">
       <c r="A362" t="s">
         <v>12</v>
       </c>
@@ -23081,7 +23224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="368" spans="1:6" customFormat="1">
+    <row r="368" spans="1:6" customFormat="1" hidden="1">
       <c r="A368" t="s">
         <v>12</v>
       </c>
@@ -23281,7 +23424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="378" spans="1:6" customFormat="1">
+    <row r="378" spans="1:6" customFormat="1" hidden="1">
       <c r="A378" t="s">
         <v>12</v>
       </c>
@@ -23381,7 +23524,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="383" spans="1:6" customFormat="1">
+    <row r="383" spans="1:6" customFormat="1" hidden="1">
       <c r="A383" t="s">
         <v>12</v>
       </c>
@@ -23561,7 +23704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="392" spans="1:6" customFormat="1">
+    <row r="392" spans="1:6" customFormat="1" hidden="1">
       <c r="A392" t="s">
         <v>13</v>
       </c>
@@ -23681,7 +23824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="398" spans="1:6" customFormat="1">
+    <row r="398" spans="1:6" customFormat="1" hidden="1">
       <c r="A398" t="s">
         <v>13</v>
       </c>
@@ -23881,7 +24024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="408" spans="1:6" customFormat="1">
+    <row r="408" spans="1:6" customFormat="1" hidden="1">
       <c r="A408" t="s">
         <v>13</v>
       </c>
@@ -23981,7 +24124,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="413" spans="1:6" customFormat="1">
+    <row r="413" spans="1:6" customFormat="1" hidden="1">
       <c r="A413" t="s">
         <v>13</v>
       </c>
@@ -24161,7 +24304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="422" spans="1:6" customFormat="1">
+    <row r="422" spans="1:6" customFormat="1" hidden="1">
       <c r="A422" t="s">
         <v>14</v>
       </c>
@@ -24281,7 +24424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="428" spans="1:6" customFormat="1">
+    <row r="428" spans="1:6" customFormat="1" hidden="1">
       <c r="A428" t="s">
         <v>14</v>
       </c>
@@ -24481,7 +24624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="438" spans="1:6" customFormat="1">
+    <row r="438" spans="1:6" customFormat="1" hidden="1">
       <c r="A438" t="s">
         <v>14</v>
       </c>
@@ -24581,7 +24724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="443" spans="1:6" customFormat="1">
+    <row r="443" spans="1:6" customFormat="1" hidden="1">
       <c r="A443" t="s">
         <v>14</v>
       </c>
@@ -24761,7 +24904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="452" spans="1:6" customFormat="1">
+    <row r="452" spans="1:6" customFormat="1" hidden="1">
       <c r="A452" t="s">
         <v>15</v>
       </c>
@@ -24881,7 +25024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="458" spans="1:6" customFormat="1">
+    <row r="458" spans="1:6" customFormat="1" hidden="1">
       <c r="A458" t="s">
         <v>15</v>
       </c>
@@ -25081,7 +25224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="468" spans="1:6" customFormat="1">
+    <row r="468" spans="1:6" customFormat="1" hidden="1">
       <c r="A468" t="s">
         <v>15</v>
       </c>
@@ -25181,7 +25324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="473" spans="1:6" customFormat="1">
+    <row r="473" spans="1:6" customFormat="1" hidden="1">
       <c r="A473" t="s">
         <v>15</v>
       </c>
@@ -25361,7 +25504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="482" spans="1:6" customFormat="1">
+    <row r="482" spans="1:6" customFormat="1" hidden="1">
       <c r="A482" t="s">
         <v>16</v>
       </c>
@@ -25481,7 +25624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="488" spans="1:6" customFormat="1">
+    <row r="488" spans="1:6" customFormat="1" hidden="1">
       <c r="A488" t="s">
         <v>16</v>
       </c>
@@ -25681,7 +25824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="498" spans="1:6" customFormat="1">
+    <row r="498" spans="1:6" customFormat="1" hidden="1">
       <c r="A498" t="s">
         <v>16</v>
       </c>
@@ -25781,7 +25924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="503" spans="1:6" customFormat="1">
+    <row r="503" spans="1:6" customFormat="1" hidden="1">
       <c r="A503" t="s">
         <v>16</v>
       </c>
@@ -25961,7 +26104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="512" spans="1:6" customFormat="1">
+    <row r="512" spans="1:6" customFormat="1" hidden="1">
       <c r="A512" t="s">
         <v>17</v>
       </c>
@@ -26081,7 +26224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="518" spans="1:6" customFormat="1">
+    <row r="518" spans="1:6" customFormat="1" hidden="1">
       <c r="A518" t="s">
         <v>17</v>
       </c>
@@ -26281,7 +26424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="528" spans="1:6" customFormat="1">
+    <row r="528" spans="1:6" customFormat="1" hidden="1">
       <c r="A528" t="s">
         <v>17</v>
       </c>
@@ -26385,7 +26528,7 @@
       </c>
       <c r="G532"/>
     </row>
-    <row r="533" spans="1:7">
+    <row r="533" spans="1:7" hidden="1">
       <c r="A533" t="s">
         <v>17</v>
       </c>
@@ -26574,7 +26717,7 @@
       </c>
       <c r="G541"/>
     </row>
-    <row r="542" spans="1:7">
+    <row r="542" spans="1:7" hidden="1">
       <c r="A542" t="s">
         <v>6</v>
       </c>
@@ -26595,7 +26738,7 @@
       </c>
       <c r="G542"/>
     </row>
-    <row r="543" spans="1:7">
+    <row r="543" spans="1:7" hidden="1">
       <c r="A543" t="s">
         <v>10</v>
       </c>
@@ -26616,7 +26759,7 @@
       </c>
       <c r="G543"/>
     </row>
-    <row r="544" spans="1:7">
+    <row r="544" spans="1:7" hidden="1">
       <c r="A544" t="s">
         <v>11</v>
       </c>
@@ -26637,7 +26780,7 @@
       </c>
       <c r="G544"/>
     </row>
-    <row r="545" spans="1:7">
+    <row r="545" spans="1:7" hidden="1">
       <c r="A545" t="s">
         <v>12</v>
       </c>
@@ -26658,7 +26801,7 @@
       </c>
       <c r="G545"/>
     </row>
-    <row r="546" spans="1:7">
+    <row r="546" spans="1:7" hidden="1">
       <c r="A546" t="s">
         <v>13</v>
       </c>
@@ -26679,7 +26822,7 @@
       </c>
       <c r="G546"/>
     </row>
-    <row r="547" spans="1:7">
+    <row r="547" spans="1:7" hidden="1">
       <c r="A547" t="s">
         <v>14</v>
       </c>
@@ -26700,7 +26843,7 @@
       </c>
       <c r="G547"/>
     </row>
-    <row r="548" spans="1:7">
+    <row r="548" spans="1:7" hidden="1">
       <c r="A548" t="s">
         <v>15</v>
       </c>
@@ -26721,7 +26864,7 @@
       </c>
       <c r="G548"/>
     </row>
-    <row r="549" spans="1:7">
+    <row r="549" spans="1:7" hidden="1">
       <c r="A549" t="s">
         <v>16</v>
       </c>
@@ -26742,7 +26885,7 @@
       </c>
       <c r="G549"/>
     </row>
-    <row r="550" spans="1:7">
+    <row r="550" spans="1:7" hidden="1">
       <c r="A550" t="s">
         <v>17</v>
       </c>
@@ -27519,7 +27662,7 @@
       </c>
       <c r="G586"/>
     </row>
-    <row r="587" spans="1:7">
+    <row r="587" spans="1:7" hidden="1">
       <c r="A587" t="s">
         <v>6</v>
       </c>
@@ -27540,7 +27683,7 @@
       </c>
       <c r="G587"/>
     </row>
-    <row r="588" spans="1:7">
+    <row r="588" spans="1:7" hidden="1">
       <c r="A588" t="s">
         <v>10</v>
       </c>
@@ -27561,7 +27704,7 @@
       </c>
       <c r="G588"/>
     </row>
-    <row r="589" spans="1:7">
+    <row r="589" spans="1:7" hidden="1">
       <c r="A589" t="s">
         <v>11</v>
       </c>
@@ -27582,7 +27725,7 @@
       </c>
       <c r="G589"/>
     </row>
-    <row r="590" spans="1:7">
+    <row r="590" spans="1:7" hidden="1">
       <c r="A590" t="s">
         <v>12</v>
       </c>
@@ -27603,7 +27746,7 @@
       </c>
       <c r="G590"/>
     </row>
-    <row r="591" spans="1:7">
+    <row r="591" spans="1:7" hidden="1">
       <c r="A591" t="s">
         <v>13</v>
       </c>
@@ -27624,7 +27767,7 @@
       </c>
       <c r="G591"/>
     </row>
-    <row r="592" spans="1:7">
+    <row r="592" spans="1:7" hidden="1">
       <c r="A592" t="s">
         <v>14</v>
       </c>
@@ -27645,7 +27788,7 @@
       </c>
       <c r="G592"/>
     </row>
-    <row r="593" spans="1:7">
+    <row r="593" spans="1:7" hidden="1">
       <c r="A593" t="s">
         <v>15</v>
       </c>
@@ -27666,7 +27809,7 @@
       </c>
       <c r="G593"/>
     </row>
-    <row r="594" spans="1:7">
+    <row r="594" spans="1:7" hidden="1">
       <c r="A594" t="s">
         <v>16</v>
       </c>
@@ -27687,7 +27830,7 @@
       </c>
       <c r="G594"/>
     </row>
-    <row r="595" spans="1:7">
+    <row r="595" spans="1:7" hidden="1">
       <c r="A595" t="s">
         <v>17</v>
       </c>
@@ -28464,7 +28607,7 @@
       </c>
       <c r="G631"/>
     </row>
-    <row r="632" spans="1:7">
+    <row r="632" spans="1:7" hidden="1">
       <c r="A632" t="s">
         <v>6</v>
       </c>
@@ -28485,7 +28628,7 @@
       </c>
       <c r="G632"/>
     </row>
-    <row r="633" spans="1:7">
+    <row r="633" spans="1:7" hidden="1">
       <c r="A633" t="s">
         <v>10</v>
       </c>
@@ -28506,7 +28649,7 @@
       </c>
       <c r="G633"/>
     </row>
-    <row r="634" spans="1:7">
+    <row r="634" spans="1:7" hidden="1">
       <c r="A634" t="s">
         <v>11</v>
       </c>
@@ -28527,7 +28670,7 @@
       </c>
       <c r="G634"/>
     </row>
-    <row r="635" spans="1:7">
+    <row r="635" spans="1:7" hidden="1">
       <c r="A635" t="s">
         <v>12</v>
       </c>
@@ -28548,7 +28691,7 @@
       </c>
       <c r="G635"/>
     </row>
-    <row r="636" spans="1:7">
+    <row r="636" spans="1:7" hidden="1">
       <c r="A636" t="s">
         <v>13</v>
       </c>
@@ -28569,7 +28712,7 @@
       </c>
       <c r="G636"/>
     </row>
-    <row r="637" spans="1:7">
+    <row r="637" spans="1:7" hidden="1">
       <c r="A637" t="s">
         <v>14</v>
       </c>
@@ -28590,7 +28733,7 @@
       </c>
       <c r="G637"/>
     </row>
-    <row r="638" spans="1:7">
+    <row r="638" spans="1:7" hidden="1">
       <c r="A638" t="s">
         <v>15</v>
       </c>
@@ -28611,7 +28754,7 @@
       </c>
       <c r="G638"/>
     </row>
-    <row r="639" spans="1:7">
+    <row r="639" spans="1:7" hidden="1">
       <c r="A639" t="s">
         <v>16</v>
       </c>
@@ -28632,7 +28775,7 @@
       </c>
       <c r="G639"/>
     </row>
-    <row r="640" spans="1:7">
+    <row r="640" spans="1:7" hidden="1">
       <c r="A640" t="s">
         <v>17</v>
       </c>
@@ -29419,7 +29562,7 @@
       <c r="C677" s="5">
         <v>2005</v>
       </c>
-      <c r="D677" s="5">
+      <c r="D677">
         <v>2.8274137896900702</v>
       </c>
       <c r="E677" s="5" t="s">
@@ -29439,7 +29582,7 @@
       <c r="C678" s="5">
         <v>2010</v>
       </c>
-      <c r="D678" s="5">
+      <c r="D678">
         <v>2.8274137896900702</v>
       </c>
       <c r="E678" s="5" t="s">
@@ -29459,7 +29602,7 @@
       <c r="C679" s="5">
         <v>2015</v>
       </c>
-      <c r="D679" s="5">
+      <c r="D679">
         <v>2.8274137896900702</v>
       </c>
       <c r="E679" s="5" t="s">
@@ -29479,7 +29622,7 @@
       <c r="C680" s="5">
         <v>2005</v>
       </c>
-      <c r="D680" s="5">
+      <c r="D680">
         <v>3.4639106615238799</v>
       </c>
       <c r="E680" s="5" t="s">
@@ -29499,7 +29642,7 @@
       <c r="C681" s="5">
         <v>2010</v>
       </c>
-      <c r="D681" s="5">
+      <c r="D681">
         <v>3.4639106615238799</v>
       </c>
       <c r="E681" s="5" t="s">
@@ -29519,7 +29662,7 @@
       <c r="C682" s="5">
         <v>2015</v>
       </c>
-      <c r="D682" s="5">
+      <c r="D682">
         <v>3.4639106615238799</v>
       </c>
       <c r="E682" s="5" t="s">
@@ -29539,7 +29682,7 @@
       <c r="C683" s="5">
         <v>2005</v>
       </c>
-      <c r="D683" s="5">
+      <c r="D683">
         <v>3.5266421098875802</v>
       </c>
       <c r="E683" s="5" t="s">
@@ -29559,7 +29702,7 @@
       <c r="C684" s="5">
         <v>2010</v>
       </c>
-      <c r="D684" s="5">
+      <c r="D684">
         <v>3.5266421098875802</v>
       </c>
       <c r="E684" s="5" t="s">
@@ -29579,7 +29722,7 @@
       <c r="C685" s="5">
         <v>2015</v>
       </c>
-      <c r="D685" s="5">
+      <c r="D685">
         <v>3.5266421098875802</v>
       </c>
       <c r="E685" s="5" t="s">
@@ -29599,7 +29742,7 @@
       <c r="C686" s="5">
         <v>2005</v>
       </c>
-      <c r="D686" s="5">
+      <c r="D686">
         <v>1.39135059941274</v>
       </c>
       <c r="E686" s="5" t="s">
@@ -29619,7 +29762,7 @@
       <c r="C687" s="5">
         <v>2010</v>
       </c>
-      <c r="D687" s="5">
+      <c r="D687">
         <v>1.39135059941274</v>
       </c>
       <c r="E687" s="5" t="s">
@@ -29639,7 +29782,7 @@
       <c r="C688" s="5">
         <v>2015</v>
       </c>
-      <c r="D688" s="5">
+      <c r="D688">
         <v>1.39135059941274</v>
       </c>
       <c r="E688" s="5" t="s">
@@ -29659,7 +29802,7 @@
       <c r="C689" s="5">
         <v>2005</v>
       </c>
-      <c r="D689" s="5">
+      <c r="D689">
         <v>1.2151303931116899</v>
       </c>
       <c r="E689" s="5" t="s">
@@ -29679,7 +29822,7 @@
       <c r="C690" s="5">
         <v>2010</v>
       </c>
-      <c r="D690" s="5">
+      <c r="D690">
         <v>1.2151303931116899</v>
       </c>
       <c r="E690" s="5" t="s">
@@ -29699,7 +29842,7 @@
       <c r="C691" s="5">
         <v>2015</v>
       </c>
-      <c r="D691" s="5">
+      <c r="D691">
         <v>1.2151303931116899</v>
       </c>
       <c r="E691" s="5" t="s">
@@ -29719,7 +29862,7 @@
       <c r="C692" s="5">
         <v>2005</v>
       </c>
-      <c r="D692" s="5">
+      <c r="D692">
         <v>4.1872025601742902</v>
       </c>
       <c r="E692" s="5" t="s">
@@ -29739,7 +29882,7 @@
       <c r="C693" s="5">
         <v>2010</v>
       </c>
-      <c r="D693" s="5">
+      <c r="D693">
         <v>4.1872025601742902</v>
       </c>
       <c r="E693" s="5" t="s">
@@ -29759,7 +29902,7 @@
       <c r="C694" s="5">
         <v>2015</v>
       </c>
-      <c r="D694" s="5">
+      <c r="D694">
         <v>4.1872025601742902</v>
       </c>
       <c r="E694" s="5" t="s">
@@ -29779,7 +29922,7 @@
       <c r="C695" s="5">
         <v>2005</v>
       </c>
-      <c r="D695" s="5">
+      <c r="D695">
         <v>5.73110199299831</v>
       </c>
       <c r="E695" s="5" t="s">
@@ -29799,7 +29942,7 @@
       <c r="C696" s="5">
         <v>2010</v>
       </c>
-      <c r="D696" s="5">
+      <c r="D696">
         <v>5.73110199299831</v>
       </c>
       <c r="E696" s="5" t="s">
@@ -29819,7 +29962,7 @@
       <c r="C697" s="5">
         <v>2015</v>
       </c>
-      <c r="D697" s="5">
+      <c r="D697">
         <v>5.73110199299831</v>
       </c>
       <c r="E697" s="5" t="s">
@@ -29839,7 +29982,7 @@
       <c r="C698" s="5">
         <v>2005</v>
       </c>
-      <c r="D698" s="5">
+      <c r="D698">
         <v>1.9515730522953301</v>
       </c>
       <c r="E698" s="5" t="s">
@@ -29859,7 +30002,7 @@
       <c r="C699" s="5">
         <v>2010</v>
       </c>
-      <c r="D699" s="5">
+      <c r="D699">
         <v>1.9515730522953301</v>
       </c>
       <c r="E699" s="5" t="s">
@@ -29879,7 +30022,7 @@
       <c r="C700" s="5">
         <v>2015</v>
       </c>
-      <c r="D700" s="5">
+      <c r="D700">
         <v>1.9515730522953301</v>
       </c>
       <c r="E700" s="5" t="s">
@@ -29899,7 +30042,7 @@
       <c r="C701" s="5">
         <v>2005</v>
       </c>
-      <c r="D701" s="5">
+      <c r="D701">
         <v>3.7006243651556199</v>
       </c>
       <c r="E701" s="5" t="s">
@@ -29919,7 +30062,7 @@
       <c r="C702" s="5">
         <v>2010</v>
       </c>
-      <c r="D702" s="5">
+      <c r="D702">
         <v>3.7006243651556199</v>
       </c>
       <c r="E702" s="5" t="s">
@@ -29939,7 +30082,7 @@
       <c r="C703" s="5">
         <v>2015</v>
       </c>
-      <c r="D703" s="5">
+      <c r="D703">
         <v>3.7006243651556199</v>
       </c>
       <c r="E703" s="5" t="s">
@@ -30003,7 +30146,7 @@
     <row r="721" spans="1:7" hidden="1">
       <c r="G721"/>
     </row>
-    <row r="722" spans="1:7">
+    <row r="722" spans="1:7" hidden="1">
       <c r="A722" t="s">
         <v>6</v>
       </c>
@@ -30024,7 +30167,7 @@
       </c>
       <c r="G722"/>
     </row>
-    <row r="723" spans="1:7">
+    <row r="723" spans="1:7" hidden="1">
       <c r="A723" t="s">
         <v>10</v>
       </c>
@@ -30045,7 +30188,7 @@
       </c>
       <c r="G723"/>
     </row>
-    <row r="724" spans="1:7">
+    <row r="724" spans="1:7" hidden="1">
       <c r="A724" t="s">
         <v>11</v>
       </c>
@@ -30066,7 +30209,7 @@
       </c>
       <c r="G724"/>
     </row>
-    <row r="725" spans="1:7">
+    <row r="725" spans="1:7" hidden="1">
       <c r="A725" t="s">
         <v>12</v>
       </c>
@@ -30087,7 +30230,7 @@
       </c>
       <c r="G725"/>
     </row>
-    <row r="726" spans="1:7">
+    <row r="726" spans="1:7" hidden="1">
       <c r="A726" t="s">
         <v>13</v>
       </c>
@@ -30108,7 +30251,7 @@
       </c>
       <c r="G726"/>
     </row>
-    <row r="727" spans="1:7">
+    <row r="727" spans="1:7" hidden="1">
       <c r="A727" t="s">
         <v>14</v>
       </c>
@@ -30129,7 +30272,7 @@
       </c>
       <c r="G727"/>
     </row>
-    <row r="728" spans="1:7">
+    <row r="728" spans="1:7" hidden="1">
       <c r="A728" t="s">
         <v>15</v>
       </c>
@@ -30150,7 +30293,7 @@
       </c>
       <c r="G728"/>
     </row>
-    <row r="729" spans="1:7">
+    <row r="729" spans="1:7" hidden="1">
       <c r="A729" t="s">
         <v>16</v>
       </c>
@@ -30171,7 +30314,7 @@
       </c>
       <c r="G729"/>
     </row>
-    <row r="730" spans="1:7">
+    <row r="730" spans="1:7" hidden="1">
       <c r="A730" t="s">
         <v>17</v>
       </c>
@@ -30759,7 +30902,7 @@
       </c>
       <c r="G757"/>
     </row>
-    <row r="758" spans="1:7">
+    <row r="758" spans="1:7" hidden="1">
       <c r="A758" t="s">
         <v>6</v>
       </c>
@@ -30780,7 +30923,7 @@
       </c>
       <c r="G758"/>
     </row>
-    <row r="759" spans="1:7">
+    <row r="759" spans="1:7" hidden="1">
       <c r="A759" t="s">
         <v>10</v>
       </c>
@@ -30801,7 +30944,7 @@
       </c>
       <c r="G759"/>
     </row>
-    <row r="760" spans="1:7">
+    <row r="760" spans="1:7" hidden="1">
       <c r="A760" t="s">
         <v>11</v>
       </c>
@@ -30822,7 +30965,7 @@
       </c>
       <c r="G760"/>
     </row>
-    <row r="761" spans="1:7">
+    <row r="761" spans="1:7" hidden="1">
       <c r="A761" t="s">
         <v>12</v>
       </c>
@@ -30843,7 +30986,7 @@
       </c>
       <c r="G761"/>
     </row>
-    <row r="762" spans="1:7">
+    <row r="762" spans="1:7" hidden="1">
       <c r="A762" t="s">
         <v>13</v>
       </c>
@@ -30864,7 +31007,7 @@
       </c>
       <c r="G762"/>
     </row>
-    <row r="763" spans="1:7">
+    <row r="763" spans="1:7" hidden="1">
       <c r="A763" t="s">
         <v>14</v>
       </c>
@@ -30885,7 +31028,7 @@
       </c>
       <c r="G763"/>
     </row>
-    <row r="764" spans="1:7">
+    <row r="764" spans="1:7" hidden="1">
       <c r="A764" t="s">
         <v>15</v>
       </c>
@@ -30906,7 +31049,7 @@
       </c>
       <c r="G764"/>
     </row>
-    <row r="765" spans="1:7">
+    <row r="765" spans="1:7" hidden="1">
       <c r="A765" t="s">
         <v>16</v>
       </c>
@@ -30927,7 +31070,7 @@
       </c>
       <c r="G765"/>
     </row>
-    <row r="766" spans="1:7">
+    <row r="766" spans="1:7" hidden="1">
       <c r="A766" t="s">
         <v>17</v>
       </c>
@@ -31893,7 +32036,7 @@
       </c>
       <c r="G811"/>
     </row>
-    <row r="812" spans="1:7">
+    <row r="812" spans="1:7" hidden="1">
       <c r="A812" t="s">
         <v>6</v>
       </c>
@@ -31914,7 +32057,7 @@
       </c>
       <c r="G812"/>
     </row>
-    <row r="813" spans="1:7">
+    <row r="813" spans="1:7" hidden="1">
       <c r="A813" t="s">
         <v>10</v>
       </c>
@@ -31935,7 +32078,7 @@
       </c>
       <c r="G813"/>
     </row>
-    <row r="814" spans="1:7">
+    <row r="814" spans="1:7" hidden="1">
       <c r="A814" t="s">
         <v>11</v>
       </c>
@@ -31956,7 +32099,7 @@
       </c>
       <c r="G814"/>
     </row>
-    <row r="815" spans="1:7">
+    <row r="815" spans="1:7" hidden="1">
       <c r="A815" t="s">
         <v>12</v>
       </c>
@@ -31977,7 +32120,7 @@
       </c>
       <c r="G815"/>
     </row>
-    <row r="816" spans="1:7">
+    <row r="816" spans="1:7" hidden="1">
       <c r="A816" t="s">
         <v>13</v>
       </c>
@@ -31998,7 +32141,7 @@
       </c>
       <c r="G816"/>
     </row>
-    <row r="817" spans="1:7">
+    <row r="817" spans="1:7" hidden="1">
       <c r="A817" t="s">
         <v>14</v>
       </c>
@@ -32019,7 +32162,7 @@
       </c>
       <c r="G817"/>
     </row>
-    <row r="818" spans="1:7">
+    <row r="818" spans="1:7" hidden="1">
       <c r="A818" t="s">
         <v>15</v>
       </c>
@@ -32040,7 +32183,7 @@
       </c>
       <c r="G818"/>
     </row>
-    <row r="819" spans="1:7">
+    <row r="819" spans="1:7" hidden="1">
       <c r="A819" t="s">
         <v>16</v>
       </c>
@@ -32061,7 +32204,7 @@
       </c>
       <c r="G819"/>
     </row>
-    <row r="820" spans="1:7">
+    <row r="820" spans="1:7" hidden="1">
       <c r="A820" t="s">
         <v>17</v>
       </c>
@@ -32460,7 +32603,7 @@
       </c>
       <c r="G838"/>
     </row>
-    <row r="839" spans="1:7">
+    <row r="839" spans="1:7" hidden="1">
       <c r="A839" t="s">
         <v>6</v>
       </c>
@@ -32481,7 +32624,7 @@
       </c>
       <c r="G839"/>
     </row>
-    <row r="840" spans="1:7">
+    <row r="840" spans="1:7" hidden="1">
       <c r="A840" t="s">
         <v>10</v>
       </c>
@@ -32502,7 +32645,7 @@
       </c>
       <c r="G840"/>
     </row>
-    <row r="841" spans="1:7">
+    <row r="841" spans="1:7" hidden="1">
       <c r="A841" t="s">
         <v>11</v>
       </c>
@@ -32523,7 +32666,7 @@
       </c>
       <c r="G841"/>
     </row>
-    <row r="842" spans="1:7">
+    <row r="842" spans="1:7" hidden="1">
       <c r="A842" t="s">
         <v>12</v>
       </c>
@@ -32544,7 +32687,7 @@
       </c>
       <c r="G842"/>
     </row>
-    <row r="843" spans="1:7">
+    <row r="843" spans="1:7" hidden="1">
       <c r="A843" t="s">
         <v>13</v>
       </c>
@@ -32565,7 +32708,7 @@
       </c>
       <c r="G843"/>
     </row>
-    <row r="844" spans="1:7">
+    <row r="844" spans="1:7" hidden="1">
       <c r="A844" t="s">
         <v>14</v>
       </c>
@@ -32586,7 +32729,7 @@
       </c>
       <c r="G844"/>
     </row>
-    <row r="845" spans="1:7">
+    <row r="845" spans="1:7" hidden="1">
       <c r="A845" t="s">
         <v>15</v>
       </c>
@@ -32607,7 +32750,7 @@
       </c>
       <c r="G845"/>
     </row>
-    <row r="846" spans="1:7">
+    <row r="846" spans="1:7" hidden="1">
       <c r="A846" t="s">
         <v>16</v>
       </c>
@@ -32628,7 +32771,7 @@
       </c>
       <c r="G846"/>
     </row>
-    <row r="847" spans="1:7">
+    <row r="847" spans="1:7" hidden="1">
       <c r="A847" t="s">
         <v>17</v>
       </c>
@@ -44577,7 +44720,7 @@
       </c>
       <c r="G1415"/>
     </row>
-    <row r="1416" spans="1:7" hidden="1">
+    <row r="1416" spans="1:7">
       <c r="A1416" t="s">
         <v>6</v>
       </c>
@@ -44598,7 +44741,7 @@
       </c>
       <c r="G1416"/>
     </row>
-    <row r="1417" spans="1:7" hidden="1">
+    <row r="1417" spans="1:7">
       <c r="A1417" t="s">
         <v>6</v>
       </c>
@@ -44619,7 +44762,7 @@
       </c>
       <c r="G1417"/>
     </row>
-    <row r="1418" spans="1:7" hidden="1">
+    <row r="1418" spans="1:7">
       <c r="A1418" t="s">
         <v>10</v>
       </c>
@@ -44640,7 +44783,7 @@
       </c>
       <c r="G1418"/>
     </row>
-    <row r="1419" spans="1:7" hidden="1">
+    <row r="1419" spans="1:7">
       <c r="A1419" t="s">
         <v>10</v>
       </c>
@@ -44661,7 +44804,7 @@
       </c>
       <c r="G1419"/>
     </row>
-    <row r="1420" spans="1:7" hidden="1">
+    <row r="1420" spans="1:7">
       <c r="A1420" t="s">
         <v>11</v>
       </c>
@@ -44682,7 +44825,7 @@
       </c>
       <c r="G1420"/>
     </row>
-    <row r="1421" spans="1:7" hidden="1">
+    <row r="1421" spans="1:7">
       <c r="A1421" t="s">
         <v>11</v>
       </c>
@@ -44703,7 +44846,7 @@
       </c>
       <c r="G1421"/>
     </row>
-    <row r="1422" spans="1:7" hidden="1">
+    <row r="1422" spans="1:7">
       <c r="A1422" t="s">
         <v>13</v>
       </c>
@@ -44724,7 +44867,7 @@
       </c>
       <c r="G1422"/>
     </row>
-    <row r="1423" spans="1:7" hidden="1">
+    <row r="1423" spans="1:7">
       <c r="A1423" t="s">
         <v>13</v>
       </c>
@@ -44745,7 +44888,7 @@
       </c>
       <c r="G1423"/>
     </row>
-    <row r="1424" spans="1:7" hidden="1">
+    <row r="1424" spans="1:7">
       <c r="A1424" t="s">
         <v>14</v>
       </c>
@@ -44766,7 +44909,7 @@
       </c>
       <c r="G1424"/>
     </row>
-    <row r="1425" spans="1:7" hidden="1">
+    <row r="1425" spans="1:7">
       <c r="A1425" t="s">
         <v>14</v>
       </c>
@@ -44787,7 +44930,7 @@
       </c>
       <c r="G1425"/>
     </row>
-    <row r="1426" spans="1:7" hidden="1">
+    <row r="1426" spans="1:7">
       <c r="A1426" t="s">
         <v>12</v>
       </c>
@@ -44808,7 +44951,7 @@
       </c>
       <c r="G1426"/>
     </row>
-    <row r="1427" spans="1:7" hidden="1">
+    <row r="1427" spans="1:7">
       <c r="A1427" t="s">
         <v>12</v>
       </c>
@@ -44829,7 +44972,7 @@
       </c>
       <c r="G1427"/>
     </row>
-    <row r="1428" spans="1:7" hidden="1">
+    <row r="1428" spans="1:7">
       <c r="A1428" t="s">
         <v>15</v>
       </c>
@@ -44850,7 +44993,7 @@
       </c>
       <c r="G1428"/>
     </row>
-    <row r="1429" spans="1:7" hidden="1">
+    <row r="1429" spans="1:7">
       <c r="A1429" t="s">
         <v>15</v>
       </c>
@@ -44871,7 +45014,7 @@
       </c>
       <c r="G1429"/>
     </row>
-    <row r="1430" spans="1:7" hidden="1">
+    <row r="1430" spans="1:7">
       <c r="A1430" t="s">
         <v>16</v>
       </c>
@@ -44892,7 +45035,7 @@
       </c>
       <c r="G1430"/>
     </row>
-    <row r="1431" spans="1:7" hidden="1">
+    <row r="1431" spans="1:7">
       <c r="A1431" t="s">
         <v>16</v>
       </c>
@@ -44913,7 +45056,7 @@
       </c>
       <c r="G1431"/>
     </row>
-    <row r="1432" spans="1:7" hidden="1">
+    <row r="1432" spans="1:7">
       <c r="A1432" t="s">
         <v>17</v>
       </c>
@@ -44934,7 +45077,7 @@
       </c>
       <c r="G1432"/>
     </row>
-    <row r="1433" spans="1:7" hidden="1">
+    <row r="1433" spans="1:7">
       <c r="A1433" t="s">
         <v>17</v>
       </c>
@@ -44955,7 +45098,7 @@
       </c>
       <c r="G1433"/>
     </row>
-    <row r="1434" spans="1:7">
+    <row r="1434" spans="1:7" hidden="1">
       <c r="A1434" s="5" t="s">
         <v>6</v>
       </c>
@@ -44976,7 +45119,7 @@
       </c>
       <c r="G1434"/>
     </row>
-    <row r="1435" spans="1:7">
+    <row r="1435" spans="1:7" hidden="1">
       <c r="A1435" s="5" t="s">
         <v>6</v>
       </c>
@@ -44997,7 +45140,7 @@
       </c>
       <c r="G1435"/>
     </row>
-    <row r="1436" spans="1:7">
+    <row r="1436" spans="1:7" hidden="1">
       <c r="A1436" s="5" t="s">
         <v>10</v>
       </c>
@@ -45018,7 +45161,7 @@
       </c>
       <c r="G1436"/>
     </row>
-    <row r="1437" spans="1:7">
+    <row r="1437" spans="1:7" hidden="1">
       <c r="A1437" s="5" t="s">
         <v>10</v>
       </c>
@@ -45039,7 +45182,7 @@
       </c>
       <c r="G1437"/>
     </row>
-    <row r="1438" spans="1:7">
+    <row r="1438" spans="1:7" hidden="1">
       <c r="A1438" s="5" t="s">
         <v>11</v>
       </c>
@@ -45060,7 +45203,7 @@
       </c>
       <c r="G1438"/>
     </row>
-    <row r="1439" spans="1:7">
+    <row r="1439" spans="1:7" hidden="1">
       <c r="A1439" s="5" t="s">
         <v>11</v>
       </c>
@@ -45081,7 +45224,7 @@
       </c>
       <c r="G1439"/>
     </row>
-    <row r="1440" spans="1:7">
+    <row r="1440" spans="1:7" hidden="1">
       <c r="A1440" s="5" t="s">
         <v>12</v>
       </c>
@@ -45102,7 +45245,7 @@
       </c>
       <c r="G1440"/>
     </row>
-    <row r="1441" spans="1:7">
+    <row r="1441" spans="1:7" hidden="1">
       <c r="A1441" s="5" t="s">
         <v>12</v>
       </c>
@@ -45123,7 +45266,7 @@
       </c>
       <c r="G1441"/>
     </row>
-    <row r="1442" spans="1:7">
+    <row r="1442" spans="1:7" hidden="1">
       <c r="A1442" s="5" t="s">
         <v>13</v>
       </c>
@@ -45144,7 +45287,7 @@
       </c>
       <c r="G1442"/>
     </row>
-    <row r="1443" spans="1:7">
+    <row r="1443" spans="1:7" hidden="1">
       <c r="A1443" s="5" t="s">
         <v>13</v>
       </c>
@@ -45165,7 +45308,7 @@
       </c>
       <c r="G1443"/>
     </row>
-    <row r="1444" spans="1:7">
+    <row r="1444" spans="1:7" hidden="1">
       <c r="A1444" s="5" t="s">
         <v>14</v>
       </c>
@@ -45186,7 +45329,7 @@
       </c>
       <c r="G1444"/>
     </row>
-    <row r="1445" spans="1:7">
+    <row r="1445" spans="1:7" hidden="1">
       <c r="A1445" s="5" t="s">
         <v>14</v>
       </c>
@@ -45207,7 +45350,7 @@
       </c>
       <c r="G1445"/>
     </row>
-    <row r="1446" spans="1:7">
+    <row r="1446" spans="1:7" hidden="1">
       <c r="A1446" s="5" t="s">
         <v>15</v>
       </c>
@@ -45228,7 +45371,7 @@
       </c>
       <c r="G1446"/>
     </row>
-    <row r="1447" spans="1:7">
+    <row r="1447" spans="1:7" hidden="1">
       <c r="A1447" s="5" t="s">
         <v>15</v>
       </c>
@@ -45249,7 +45392,7 @@
       </c>
       <c r="G1447"/>
     </row>
-    <row r="1448" spans="1:7">
+    <row r="1448" spans="1:7" hidden="1">
       <c r="A1448" s="5" t="s">
         <v>16</v>
       </c>
@@ -45270,7 +45413,7 @@
       </c>
       <c r="G1448"/>
     </row>
-    <row r="1449" spans="1:7">
+    <row r="1449" spans="1:7" hidden="1">
       <c r="A1449" s="5" t="s">
         <v>16</v>
       </c>
@@ -45291,7 +45434,7 @@
       </c>
       <c r="G1449"/>
     </row>
-    <row r="1450" spans="1:7">
+    <row r="1450" spans="1:7" hidden="1">
       <c r="A1450" s="5" t="s">
         <v>17</v>
       </c>
@@ -45312,7 +45455,7 @@
       </c>
       <c r="G1450"/>
     </row>
-    <row r="1451" spans="1:7">
+    <row r="1451" spans="1:7" hidden="1">
       <c r="A1451" s="5" t="s">
         <v>17</v>
       </c>
@@ -45715,14 +45858,7 @@
   <autoFilter ref="B1:B1469" xr:uid="{A58F1B57-0ED0-3247-9112-85DD1F029275}">
     <filterColumn colId="0">
       <filters>
-        <filter val="T_HDV_BS_CNG_R"/>
-        <filter val="T_HDV_BT_CNG_R"/>
-        <filter val="T_HDV_TCCNG_R"/>
-        <filter val="T_LDV_CCNG_R"/>
-        <filter val="T_LDV_FCNG_R"/>
-        <filter val="T_LDV_MVCNG_R"/>
-        <filter val="T_LDV_PCNG_R"/>
-        <filter val="T_MDV_TMCNG_R"/>
+        <filter val="T_HDV_THLDSL_R"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -45732,10 +45868,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E45044-B387-C440-9E53-EFE5C4A0945F}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -48206,7 +48342,1520 @@
       </c>
       <c r="J82" s="2"/>
     </row>
+    <row r="83" spans="1:10">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83" t="s">
+        <v>198</v>
+      </c>
+      <c r="D83" t="s">
+        <v>102</v>
+      </c>
+      <c r="E83">
+        <v>2018</v>
+      </c>
+      <c r="F83" t="s">
+        <v>199</v>
+      </c>
+      <c r="G83">
+        <v>15.32</v>
+      </c>
+      <c r="H83" t="s">
+        <v>87</v>
+      </c>
+      <c r="I83" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" t="s">
+        <v>198</v>
+      </c>
+      <c r="D84" t="s">
+        <v>102</v>
+      </c>
+      <c r="E84">
+        <v>2015</v>
+      </c>
+      <c r="F84" t="s">
+        <v>199</v>
+      </c>
+      <c r="G84">
+        <v>15.32</v>
+      </c>
+      <c r="H84" t="s">
+        <v>87</v>
+      </c>
+      <c r="I84" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" t="s">
+        <v>198</v>
+      </c>
+      <c r="D85" t="s">
+        <v>102</v>
+      </c>
+      <c r="E85">
+        <v>2018</v>
+      </c>
+      <c r="F85" t="s">
+        <v>199</v>
+      </c>
+      <c r="G85">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" t="s">
+        <v>198</v>
+      </c>
+      <c r="D86" t="s">
+        <v>102</v>
+      </c>
+      <c r="E86">
+        <v>2015</v>
+      </c>
+      <c r="F86" t="s">
+        <v>199</v>
+      </c>
+      <c r="G86">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H86" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>90</v>
+      </c>
+      <c r="C87" t="s">
+        <v>198</v>
+      </c>
+      <c r="D87" t="s">
+        <v>102</v>
+      </c>
+      <c r="E87">
+        <v>2018</v>
+      </c>
+      <c r="F87" t="s">
+        <v>199</v>
+      </c>
+      <c r="G87">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H87" t="s">
+        <v>87</v>
+      </c>
+      <c r="I87" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+      <c r="C88" t="s">
+        <v>198</v>
+      </c>
+      <c r="D88" t="s">
+        <v>102</v>
+      </c>
+      <c r="E88">
+        <v>2015</v>
+      </c>
+      <c r="F88" t="s">
+        <v>199</v>
+      </c>
+      <c r="G88">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H88" t="s">
+        <v>87</v>
+      </c>
+      <c r="I88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" t="s">
+        <v>86</v>
+      </c>
+      <c r="C89" t="s">
+        <v>198</v>
+      </c>
+      <c r="D89" t="s">
+        <v>102</v>
+      </c>
+      <c r="E89">
+        <v>2018</v>
+      </c>
+      <c r="F89" t="s">
+        <v>199</v>
+      </c>
+      <c r="G89">
+        <v>15.32</v>
+      </c>
+      <c r="H89" t="s">
+        <v>87</v>
+      </c>
+      <c r="I89" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" t="s">
+        <v>86</v>
+      </c>
+      <c r="C90" t="s">
+        <v>198</v>
+      </c>
+      <c r="D90" t="s">
+        <v>102</v>
+      </c>
+      <c r="E90">
+        <v>2015</v>
+      </c>
+      <c r="F90" t="s">
+        <v>199</v>
+      </c>
+      <c r="G90">
+        <v>15.32</v>
+      </c>
+      <c r="H90" t="s">
+        <v>87</v>
+      </c>
+      <c r="I90" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" t="s">
+        <v>89</v>
+      </c>
+      <c r="C91" t="s">
+        <v>198</v>
+      </c>
+      <c r="D91" t="s">
+        <v>102</v>
+      </c>
+      <c r="E91">
+        <v>2018</v>
+      </c>
+      <c r="F91" t="s">
+        <v>199</v>
+      </c>
+      <c r="G91">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H91" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" t="s">
+        <v>198</v>
+      </c>
+      <c r="D92" t="s">
+        <v>102</v>
+      </c>
+      <c r="E92">
+        <v>2015</v>
+      </c>
+      <c r="F92" t="s">
+        <v>199</v>
+      </c>
+      <c r="G92">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H92" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" t="s">
+        <v>198</v>
+      </c>
+      <c r="D93" t="s">
+        <v>102</v>
+      </c>
+      <c r="E93">
+        <v>2018</v>
+      </c>
+      <c r="F93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G93">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H93" t="s">
+        <v>87</v>
+      </c>
+      <c r="I93" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" t="s">
+        <v>90</v>
+      </c>
+      <c r="C94" t="s">
+        <v>198</v>
+      </c>
+      <c r="D94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E94">
+        <v>2015</v>
+      </c>
+      <c r="F94" t="s">
+        <v>199</v>
+      </c>
+      <c r="G94">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H94" t="s">
+        <v>87</v>
+      </c>
+      <c r="I94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" t="s">
+        <v>11</v>
+      </c>
+      <c r="B95" t="s">
+        <v>86</v>
+      </c>
+      <c r="C95" t="s">
+        <v>198</v>
+      </c>
+      <c r="D95" t="s">
+        <v>102</v>
+      </c>
+      <c r="E95">
+        <v>2018</v>
+      </c>
+      <c r="F95" t="s">
+        <v>199</v>
+      </c>
+      <c r="G95">
+        <v>15.32</v>
+      </c>
+      <c r="H95" t="s">
+        <v>87</v>
+      </c>
+      <c r="I95" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" t="s">
+        <v>86</v>
+      </c>
+      <c r="C96" t="s">
+        <v>198</v>
+      </c>
+      <c r="D96" t="s">
+        <v>102</v>
+      </c>
+      <c r="E96">
+        <v>2015</v>
+      </c>
+      <c r="F96" t="s">
+        <v>199</v>
+      </c>
+      <c r="G96">
+        <v>15.32</v>
+      </c>
+      <c r="H96" t="s">
+        <v>87</v>
+      </c>
+      <c r="I96" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" t="s">
+        <v>89</v>
+      </c>
+      <c r="C97" t="s">
+        <v>198</v>
+      </c>
+      <c r="D97" t="s">
+        <v>102</v>
+      </c>
+      <c r="E97">
+        <v>2018</v>
+      </c>
+      <c r="F97" t="s">
+        <v>199</v>
+      </c>
+      <c r="G97">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H97" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" t="s">
+        <v>89</v>
+      </c>
+      <c r="C98" t="s">
+        <v>198</v>
+      </c>
+      <c r="D98" t="s">
+        <v>102</v>
+      </c>
+      <c r="E98">
+        <v>2015</v>
+      </c>
+      <c r="F98" t="s">
+        <v>199</v>
+      </c>
+      <c r="G98">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" t="s">
+        <v>90</v>
+      </c>
+      <c r="C99" t="s">
+        <v>198</v>
+      </c>
+      <c r="D99" t="s">
+        <v>102</v>
+      </c>
+      <c r="E99">
+        <v>2018</v>
+      </c>
+      <c r="F99" t="s">
+        <v>199</v>
+      </c>
+      <c r="G99">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H99" t="s">
+        <v>87</v>
+      </c>
+      <c r="I99" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" t="s">
+        <v>90</v>
+      </c>
+      <c r="C100" t="s">
+        <v>198</v>
+      </c>
+      <c r="D100" t="s">
+        <v>102</v>
+      </c>
+      <c r="E100">
+        <v>2015</v>
+      </c>
+      <c r="F100" t="s">
+        <v>199</v>
+      </c>
+      <c r="G100">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H100" t="s">
+        <v>87</v>
+      </c>
+      <c r="I100" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>13</v>
+      </c>
+      <c r="B101" t="s">
+        <v>86</v>
+      </c>
+      <c r="C101" t="s">
+        <v>198</v>
+      </c>
+      <c r="D101" t="s">
+        <v>102</v>
+      </c>
+      <c r="E101">
+        <v>2018</v>
+      </c>
+      <c r="F101" t="s">
+        <v>199</v>
+      </c>
+      <c r="G101">
+        <v>15.32</v>
+      </c>
+      <c r="H101" t="s">
+        <v>87</v>
+      </c>
+      <c r="I101" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>13</v>
+      </c>
+      <c r="B102" t="s">
+        <v>86</v>
+      </c>
+      <c r="C102" t="s">
+        <v>198</v>
+      </c>
+      <c r="D102" t="s">
+        <v>102</v>
+      </c>
+      <c r="E102">
+        <v>2015</v>
+      </c>
+      <c r="F102" t="s">
+        <v>199</v>
+      </c>
+      <c r="G102">
+        <v>15.32</v>
+      </c>
+      <c r="H102" t="s">
+        <v>87</v>
+      </c>
+      <c r="I102" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>13</v>
+      </c>
+      <c r="B103" t="s">
+        <v>89</v>
+      </c>
+      <c r="C103" t="s">
+        <v>198</v>
+      </c>
+      <c r="D103" t="s">
+        <v>102</v>
+      </c>
+      <c r="E103">
+        <v>2018</v>
+      </c>
+      <c r="F103" t="s">
+        <v>199</v>
+      </c>
+      <c r="G103">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H103" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" t="s">
+        <v>89</v>
+      </c>
+      <c r="C104" t="s">
+        <v>198</v>
+      </c>
+      <c r="D104" t="s">
+        <v>102</v>
+      </c>
+      <c r="E104">
+        <v>2015</v>
+      </c>
+      <c r="F104" t="s">
+        <v>199</v>
+      </c>
+      <c r="G104">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H104" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>13</v>
+      </c>
+      <c r="B105" t="s">
+        <v>90</v>
+      </c>
+      <c r="C105" t="s">
+        <v>198</v>
+      </c>
+      <c r="D105" t="s">
+        <v>102</v>
+      </c>
+      <c r="E105">
+        <v>2018</v>
+      </c>
+      <c r="F105" t="s">
+        <v>199</v>
+      </c>
+      <c r="G105">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H105" t="s">
+        <v>87</v>
+      </c>
+      <c r="I105" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" t="s">
+        <v>90</v>
+      </c>
+      <c r="C106" t="s">
+        <v>198</v>
+      </c>
+      <c r="D106" t="s">
+        <v>102</v>
+      </c>
+      <c r="E106">
+        <v>2015</v>
+      </c>
+      <c r="F106" t="s">
+        <v>199</v>
+      </c>
+      <c r="G106">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H106" t="s">
+        <v>87</v>
+      </c>
+      <c r="I106" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" t="s">
+        <v>198</v>
+      </c>
+      <c r="D107" t="s">
+        <v>102</v>
+      </c>
+      <c r="E107">
+        <v>2018</v>
+      </c>
+      <c r="F107" t="s">
+        <v>199</v>
+      </c>
+      <c r="G107">
+        <v>15.32</v>
+      </c>
+      <c r="H107" t="s">
+        <v>87</v>
+      </c>
+      <c r="I107" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
+        <v>86</v>
+      </c>
+      <c r="C108" t="s">
+        <v>198</v>
+      </c>
+      <c r="D108" t="s">
+        <v>102</v>
+      </c>
+      <c r="E108">
+        <v>2015</v>
+      </c>
+      <c r="F108" t="s">
+        <v>199</v>
+      </c>
+      <c r="G108">
+        <v>15.32</v>
+      </c>
+      <c r="H108" t="s">
+        <v>87</v>
+      </c>
+      <c r="I108" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109" t="s">
+        <v>89</v>
+      </c>
+      <c r="C109" t="s">
+        <v>198</v>
+      </c>
+      <c r="D109" t="s">
+        <v>102</v>
+      </c>
+      <c r="E109">
+        <v>2018</v>
+      </c>
+      <c r="F109" t="s">
+        <v>199</v>
+      </c>
+      <c r="G109">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H109" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" t="s">
+        <v>89</v>
+      </c>
+      <c r="C110" t="s">
+        <v>198</v>
+      </c>
+      <c r="D110" t="s">
+        <v>102</v>
+      </c>
+      <c r="E110">
+        <v>2015</v>
+      </c>
+      <c r="F110" t="s">
+        <v>199</v>
+      </c>
+      <c r="G110">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H110" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>14</v>
+      </c>
+      <c r="B111" t="s">
+        <v>90</v>
+      </c>
+      <c r="C111" t="s">
+        <v>198</v>
+      </c>
+      <c r="D111" t="s">
+        <v>102</v>
+      </c>
+      <c r="E111">
+        <v>2018</v>
+      </c>
+      <c r="F111" t="s">
+        <v>199</v>
+      </c>
+      <c r="G111">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H111" t="s">
+        <v>87</v>
+      </c>
+      <c r="I111" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112" t="s">
+        <v>90</v>
+      </c>
+      <c r="C112" t="s">
+        <v>198</v>
+      </c>
+      <c r="D112" t="s">
+        <v>102</v>
+      </c>
+      <c r="E112">
+        <v>2015</v>
+      </c>
+      <c r="F112" t="s">
+        <v>199</v>
+      </c>
+      <c r="G112">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H112" t="s">
+        <v>87</v>
+      </c>
+      <c r="I112" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" t="s">
+        <v>86</v>
+      </c>
+      <c r="C113" t="s">
+        <v>198</v>
+      </c>
+      <c r="D113" t="s">
+        <v>102</v>
+      </c>
+      <c r="E113">
+        <v>2018</v>
+      </c>
+      <c r="F113" t="s">
+        <v>199</v>
+      </c>
+      <c r="G113">
+        <v>15.32</v>
+      </c>
+      <c r="H113" t="s">
+        <v>87</v>
+      </c>
+      <c r="I113" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" t="s">
+        <v>86</v>
+      </c>
+      <c r="C114" t="s">
+        <v>198</v>
+      </c>
+      <c r="D114" t="s">
+        <v>102</v>
+      </c>
+      <c r="E114">
+        <v>2015</v>
+      </c>
+      <c r="F114" t="s">
+        <v>199</v>
+      </c>
+      <c r="G114">
+        <v>15.32</v>
+      </c>
+      <c r="H114" t="s">
+        <v>87</v>
+      </c>
+      <c r="I114" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>12</v>
+      </c>
+      <c r="B115" t="s">
+        <v>89</v>
+      </c>
+      <c r="C115" t="s">
+        <v>198</v>
+      </c>
+      <c r="D115" t="s">
+        <v>102</v>
+      </c>
+      <c r="E115">
+        <v>2018</v>
+      </c>
+      <c r="F115" t="s">
+        <v>199</v>
+      </c>
+      <c r="G115">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H115" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116" t="s">
+        <v>89</v>
+      </c>
+      <c r="C116" t="s">
+        <v>198</v>
+      </c>
+      <c r="D116" t="s">
+        <v>102</v>
+      </c>
+      <c r="E116">
+        <v>2015</v>
+      </c>
+      <c r="F116" t="s">
+        <v>199</v>
+      </c>
+      <c r="G116">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H116" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" t="s">
+        <v>90</v>
+      </c>
+      <c r="C117" t="s">
+        <v>198</v>
+      </c>
+      <c r="D117" t="s">
+        <v>102</v>
+      </c>
+      <c r="E117">
+        <v>2018</v>
+      </c>
+      <c r="F117" t="s">
+        <v>199</v>
+      </c>
+      <c r="G117">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H117" t="s">
+        <v>87</v>
+      </c>
+      <c r="I117" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118" t="s">
+        <v>90</v>
+      </c>
+      <c r="C118" t="s">
+        <v>198</v>
+      </c>
+      <c r="D118" t="s">
+        <v>102</v>
+      </c>
+      <c r="E118">
+        <v>2015</v>
+      </c>
+      <c r="F118" t="s">
+        <v>199</v>
+      </c>
+      <c r="G118">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H118" t="s">
+        <v>87</v>
+      </c>
+      <c r="I118" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>15</v>
+      </c>
+      <c r="B119" t="s">
+        <v>86</v>
+      </c>
+      <c r="C119" t="s">
+        <v>198</v>
+      </c>
+      <c r="D119" t="s">
+        <v>102</v>
+      </c>
+      <c r="E119">
+        <v>2018</v>
+      </c>
+      <c r="F119" t="s">
+        <v>199</v>
+      </c>
+      <c r="G119">
+        <v>15.32</v>
+      </c>
+      <c r="H119" t="s">
+        <v>87</v>
+      </c>
+      <c r="I119" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>15</v>
+      </c>
+      <c r="B120" t="s">
+        <v>86</v>
+      </c>
+      <c r="C120" t="s">
+        <v>198</v>
+      </c>
+      <c r="D120" t="s">
+        <v>102</v>
+      </c>
+      <c r="E120">
+        <v>2015</v>
+      </c>
+      <c r="F120" t="s">
+        <v>199</v>
+      </c>
+      <c r="G120">
+        <v>15.32</v>
+      </c>
+      <c r="H120" t="s">
+        <v>87</v>
+      </c>
+      <c r="I120" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>15</v>
+      </c>
+      <c r="B121" t="s">
+        <v>89</v>
+      </c>
+      <c r="C121" t="s">
+        <v>198</v>
+      </c>
+      <c r="D121" t="s">
+        <v>102</v>
+      </c>
+      <c r="E121">
+        <v>2018</v>
+      </c>
+      <c r="F121" t="s">
+        <v>199</v>
+      </c>
+      <c r="G121">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H121" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>15</v>
+      </c>
+      <c r="B122" t="s">
+        <v>89</v>
+      </c>
+      <c r="C122" t="s">
+        <v>198</v>
+      </c>
+      <c r="D122" t="s">
+        <v>102</v>
+      </c>
+      <c r="E122">
+        <v>2015</v>
+      </c>
+      <c r="F122" t="s">
+        <v>199</v>
+      </c>
+      <c r="G122">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H122" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
+        <v>15</v>
+      </c>
+      <c r="B123" t="s">
+        <v>90</v>
+      </c>
+      <c r="C123" t="s">
+        <v>198</v>
+      </c>
+      <c r="D123" t="s">
+        <v>102</v>
+      </c>
+      <c r="E123">
+        <v>2018</v>
+      </c>
+      <c r="F123" t="s">
+        <v>199</v>
+      </c>
+      <c r="G123">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H123" t="s">
+        <v>87</v>
+      </c>
+      <c r="I123" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" t="s">
+        <v>15</v>
+      </c>
+      <c r="B124" t="s">
+        <v>90</v>
+      </c>
+      <c r="C124" t="s">
+        <v>198</v>
+      </c>
+      <c r="D124" t="s">
+        <v>102</v>
+      </c>
+      <c r="E124">
+        <v>2015</v>
+      </c>
+      <c r="F124" t="s">
+        <v>199</v>
+      </c>
+      <c r="G124">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H124" t="s">
+        <v>87</v>
+      </c>
+      <c r="I124" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" t="s">
+        <v>16</v>
+      </c>
+      <c r="B125" t="s">
+        <v>86</v>
+      </c>
+      <c r="C125" t="s">
+        <v>198</v>
+      </c>
+      <c r="D125" t="s">
+        <v>102</v>
+      </c>
+      <c r="E125">
+        <v>2018</v>
+      </c>
+      <c r="F125" t="s">
+        <v>199</v>
+      </c>
+      <c r="G125">
+        <v>15.32</v>
+      </c>
+      <c r="H125" t="s">
+        <v>87</v>
+      </c>
+      <c r="I125" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" t="s">
+        <v>16</v>
+      </c>
+      <c r="B126" t="s">
+        <v>86</v>
+      </c>
+      <c r="C126" t="s">
+        <v>198</v>
+      </c>
+      <c r="D126" t="s">
+        <v>102</v>
+      </c>
+      <c r="E126">
+        <v>2015</v>
+      </c>
+      <c r="F126" t="s">
+        <v>199</v>
+      </c>
+      <c r="G126">
+        <v>15.32</v>
+      </c>
+      <c r="H126" t="s">
+        <v>87</v>
+      </c>
+      <c r="I126" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" t="s">
+        <v>16</v>
+      </c>
+      <c r="B127" t="s">
+        <v>89</v>
+      </c>
+      <c r="C127" t="s">
+        <v>198</v>
+      </c>
+      <c r="D127" t="s">
+        <v>102</v>
+      </c>
+      <c r="E127">
+        <v>2018</v>
+      </c>
+      <c r="F127" t="s">
+        <v>199</v>
+      </c>
+      <c r="G127">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H127" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" t="s">
+        <v>16</v>
+      </c>
+      <c r="B128" t="s">
+        <v>89</v>
+      </c>
+      <c r="C128" t="s">
+        <v>198</v>
+      </c>
+      <c r="D128" t="s">
+        <v>102</v>
+      </c>
+      <c r="E128">
+        <v>2015</v>
+      </c>
+      <c r="F128" t="s">
+        <v>199</v>
+      </c>
+      <c r="G128">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H128" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129" t="s">
+        <v>16</v>
+      </c>
+      <c r="B129" t="s">
+        <v>90</v>
+      </c>
+      <c r="C129" t="s">
+        <v>198</v>
+      </c>
+      <c r="D129" t="s">
+        <v>102</v>
+      </c>
+      <c r="E129">
+        <v>2018</v>
+      </c>
+      <c r="F129" t="s">
+        <v>199</v>
+      </c>
+      <c r="G129">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H129" t="s">
+        <v>87</v>
+      </c>
+      <c r="I129" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130" t="s">
+        <v>16</v>
+      </c>
+      <c r="B130" t="s">
+        <v>90</v>
+      </c>
+      <c r="C130" t="s">
+        <v>198</v>
+      </c>
+      <c r="D130" t="s">
+        <v>102</v>
+      </c>
+      <c r="E130">
+        <v>2015</v>
+      </c>
+      <c r="F130" t="s">
+        <v>199</v>
+      </c>
+      <c r="G130">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H130" t="s">
+        <v>87</v>
+      </c>
+      <c r="I130" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" t="s">
+        <v>17</v>
+      </c>
+      <c r="B131" t="s">
+        <v>86</v>
+      </c>
+      <c r="C131" t="s">
+        <v>198</v>
+      </c>
+      <c r="D131" t="s">
+        <v>102</v>
+      </c>
+      <c r="E131">
+        <v>2018</v>
+      </c>
+      <c r="F131" t="s">
+        <v>199</v>
+      </c>
+      <c r="G131">
+        <v>15.32</v>
+      </c>
+      <c r="H131" t="s">
+        <v>87</v>
+      </c>
+      <c r="I131" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" t="s">
+        <v>17</v>
+      </c>
+      <c r="B132" t="s">
+        <v>86</v>
+      </c>
+      <c r="C132" t="s">
+        <v>198</v>
+      </c>
+      <c r="D132" t="s">
+        <v>102</v>
+      </c>
+      <c r="E132">
+        <v>2015</v>
+      </c>
+      <c r="F132" t="s">
+        <v>199</v>
+      </c>
+      <c r="G132">
+        <v>15.32</v>
+      </c>
+      <c r="H132" t="s">
+        <v>87</v>
+      </c>
+      <c r="I132" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" t="s">
+        <v>17</v>
+      </c>
+      <c r="B133" t="s">
+        <v>89</v>
+      </c>
+      <c r="C133" t="s">
+        <v>198</v>
+      </c>
+      <c r="D133" t="s">
+        <v>102</v>
+      </c>
+      <c r="E133">
+        <v>2018</v>
+      </c>
+      <c r="F133" t="s">
+        <v>199</v>
+      </c>
+      <c r="G133">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H133" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" t="s">
+        <v>17</v>
+      </c>
+      <c r="B134" t="s">
+        <v>89</v>
+      </c>
+      <c r="C134" t="s">
+        <v>198</v>
+      </c>
+      <c r="D134" t="s">
+        <v>102</v>
+      </c>
+      <c r="E134">
+        <v>2015</v>
+      </c>
+      <c r="F134" t="s">
+        <v>199</v>
+      </c>
+      <c r="G134">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H134" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135" t="s">
+        <v>17</v>
+      </c>
+      <c r="B135" t="s">
+        <v>90</v>
+      </c>
+      <c r="C135" t="s">
+        <v>198</v>
+      </c>
+      <c r="D135" t="s">
+        <v>102</v>
+      </c>
+      <c r="E135">
+        <v>2018</v>
+      </c>
+      <c r="F135" t="s">
+        <v>199</v>
+      </c>
+      <c r="G135">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H135" t="s">
+        <v>87</v>
+      </c>
+      <c r="I135" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" t="s">
+        <v>17</v>
+      </c>
+      <c r="B136" t="s">
+        <v>90</v>
+      </c>
+      <c r="C136" t="s">
+        <v>198</v>
+      </c>
+      <c r="D136" t="s">
+        <v>102</v>
+      </c>
+      <c r="E136">
+        <v>2015</v>
+      </c>
+      <c r="F136" t="s">
+        <v>199</v>
+      </c>
+      <c r="G136">
+        <v>1.7149999999999999E-2</v>
+      </c>
+      <c r="H136" t="s">
+        <v>87</v>
+      </c>
+      <c r="I136" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I136" xr:uid="{53A636C6-2F56-BB45-9E84-D95EC8C8B980}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -48443,10 +50092,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2737C6E4-DD82-2048-A722-D97786E2AA4E}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD19"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="Q89" sqref="Q89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -50341,6 +51990,420 @@
         <v>83</v>
       </c>
     </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>198</v>
+      </c>
+      <c r="C83" t="s">
+        <v>102</v>
+      </c>
+      <c r="D83">
+        <v>2018</v>
+      </c>
+      <c r="E83" t="s">
+        <v>199</v>
+      </c>
+      <c r="F83">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G83" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>198</v>
+      </c>
+      <c r="C84" t="s">
+        <v>102</v>
+      </c>
+      <c r="D84">
+        <v>2015</v>
+      </c>
+      <c r="E84" t="s">
+        <v>199</v>
+      </c>
+      <c r="F84">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G84" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" t="s">
+        <v>102</v>
+      </c>
+      <c r="D85">
+        <v>2018</v>
+      </c>
+      <c r="E85" t="s">
+        <v>199</v>
+      </c>
+      <c r="F85">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G85" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" t="s">
+        <v>198</v>
+      </c>
+      <c r="C86" t="s">
+        <v>102</v>
+      </c>
+      <c r="D86">
+        <v>2015</v>
+      </c>
+      <c r="E86" t="s">
+        <v>199</v>
+      </c>
+      <c r="F86">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G86" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" t="s">
+        <v>198</v>
+      </c>
+      <c r="C87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D87">
+        <v>2018</v>
+      </c>
+      <c r="E87" t="s">
+        <v>199</v>
+      </c>
+      <c r="F87">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G87" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" t="s">
+        <v>102</v>
+      </c>
+      <c r="D88">
+        <v>2015</v>
+      </c>
+      <c r="E88" t="s">
+        <v>199</v>
+      </c>
+      <c r="F88">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G88" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" t="s">
+        <v>198</v>
+      </c>
+      <c r="C89" t="s">
+        <v>102</v>
+      </c>
+      <c r="D89">
+        <v>2018</v>
+      </c>
+      <c r="E89" t="s">
+        <v>199</v>
+      </c>
+      <c r="F89">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G89" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" t="s">
+        <v>198</v>
+      </c>
+      <c r="C90" t="s">
+        <v>102</v>
+      </c>
+      <c r="D90">
+        <v>2015</v>
+      </c>
+      <c r="E90" t="s">
+        <v>199</v>
+      </c>
+      <c r="F90">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G90" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" t="s">
+        <v>198</v>
+      </c>
+      <c r="C91" t="s">
+        <v>102</v>
+      </c>
+      <c r="D91">
+        <v>2018</v>
+      </c>
+      <c r="E91" t="s">
+        <v>199</v>
+      </c>
+      <c r="F91">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G91" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" t="s">
+        <v>198</v>
+      </c>
+      <c r="C92" t="s">
+        <v>102</v>
+      </c>
+      <c r="D92">
+        <v>2015</v>
+      </c>
+      <c r="E92" t="s">
+        <v>199</v>
+      </c>
+      <c r="F92">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G92" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" t="s">
+        <v>198</v>
+      </c>
+      <c r="C93" t="s">
+        <v>102</v>
+      </c>
+      <c r="D93">
+        <v>2018</v>
+      </c>
+      <c r="E93" t="s">
+        <v>199</v>
+      </c>
+      <c r="F93">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G93" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" t="s">
+        <v>198</v>
+      </c>
+      <c r="C94" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94">
+        <v>2015</v>
+      </c>
+      <c r="E94" t="s">
+        <v>199</v>
+      </c>
+      <c r="F94">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G94" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>15</v>
+      </c>
+      <c r="B95" t="s">
+        <v>198</v>
+      </c>
+      <c r="C95" t="s">
+        <v>102</v>
+      </c>
+      <c r="D95">
+        <v>2018</v>
+      </c>
+      <c r="E95" t="s">
+        <v>199</v>
+      </c>
+      <c r="F95">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G95" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" t="s">
+        <v>198</v>
+      </c>
+      <c r="C96" t="s">
+        <v>102</v>
+      </c>
+      <c r="D96">
+        <v>2015</v>
+      </c>
+      <c r="E96" t="s">
+        <v>199</v>
+      </c>
+      <c r="F96">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G96" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B97" t="s">
+        <v>198</v>
+      </c>
+      <c r="C97" t="s">
+        <v>102</v>
+      </c>
+      <c r="D97">
+        <v>2018</v>
+      </c>
+      <c r="E97" t="s">
+        <v>199</v>
+      </c>
+      <c r="F97">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G97" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B98" t="s">
+        <v>198</v>
+      </c>
+      <c r="C98" t="s">
+        <v>102</v>
+      </c>
+      <c r="D98">
+        <v>2015</v>
+      </c>
+      <c r="E98" t="s">
+        <v>199</v>
+      </c>
+      <c r="F98">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G98" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99" t="s">
+        <v>198</v>
+      </c>
+      <c r="C99" t="s">
+        <v>102</v>
+      </c>
+      <c r="D99">
+        <v>2018</v>
+      </c>
+      <c r="E99" t="s">
+        <v>199</v>
+      </c>
+      <c r="F99">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G99" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100" t="s">
+        <v>198</v>
+      </c>
+      <c r="C100" t="s">
+        <v>102</v>
+      </c>
+      <c r="D100">
+        <v>2015</v>
+      </c>
+      <c r="E100" t="s">
+        <v>199</v>
+      </c>
+      <c r="F100">
+        <v>6.1963140526741803E-2</v>
+      </c>
+      <c r="G100" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G82" xr:uid="{2737C6E4-DD82-2048-A722-D97786E2AA4E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50348,10 +52411,465 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE438D4-1BF8-0947-90AC-2AC0B0A50AAD}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2">
+        <v>2018</v>
+      </c>
+      <c r="E2">
+        <v>152</v>
+      </c>
+      <c r="F2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
+        <v>2015</v>
+      </c>
+      <c r="E3">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
+        <v>2018</v>
+      </c>
+      <c r="E4">
+        <v>152</v>
+      </c>
+      <c r="F4" t="s">
+        <v>202</v>
+      </c>
+      <c r="G4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5">
+        <v>2015</v>
+      </c>
+      <c r="E5">
+        <v>152</v>
+      </c>
+      <c r="F5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6">
+        <v>2018</v>
+      </c>
+      <c r="E6">
+        <v>152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7">
+        <v>2015</v>
+      </c>
+      <c r="E7">
+        <v>152</v>
+      </c>
+      <c r="F7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2020</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8">
+        <v>2018</v>
+      </c>
+      <c r="E8">
+        <v>152</v>
+      </c>
+      <c r="F8" t="s">
+        <v>202</v>
+      </c>
+      <c r="G8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>2020</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9">
+        <v>2015</v>
+      </c>
+      <c r="E9">
+        <v>152</v>
+      </c>
+      <c r="F9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>2020</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10">
+        <v>2018</v>
+      </c>
+      <c r="E10">
+        <v>152</v>
+      </c>
+      <c r="F10" t="s">
+        <v>202</v>
+      </c>
+      <c r="G10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>2020</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11">
+        <v>2015</v>
+      </c>
+      <c r="E11">
+        <v>152</v>
+      </c>
+      <c r="F11" t="s">
+        <v>202</v>
+      </c>
+      <c r="G11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12">
+        <v>2018</v>
+      </c>
+      <c r="E12">
+        <v>152</v>
+      </c>
+      <c r="F12" t="s">
+        <v>202</v>
+      </c>
+      <c r="G12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2020</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13">
+        <v>2015</v>
+      </c>
+      <c r="E13">
+        <v>152</v>
+      </c>
+      <c r="F13" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>2020</v>
+      </c>
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14">
+        <v>2018</v>
+      </c>
+      <c r="E14">
+        <v>152</v>
+      </c>
+      <c r="F14" t="s">
+        <v>202</v>
+      </c>
+      <c r="G14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>2020</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15">
+        <v>2015</v>
+      </c>
+      <c r="E15">
+        <v>152</v>
+      </c>
+      <c r="F15" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>2020</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16">
+        <v>2018</v>
+      </c>
+      <c r="E16">
+        <v>152</v>
+      </c>
+      <c r="F16" t="s">
+        <v>202</v>
+      </c>
+      <c r="G16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2020</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17">
+        <v>2015</v>
+      </c>
+      <c r="E17">
+        <v>152</v>
+      </c>
+      <c r="F17" t="s">
+        <v>202</v>
+      </c>
+      <c r="G17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2020</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18">
+        <v>2018</v>
+      </c>
+      <c r="E18">
+        <v>152</v>
+      </c>
+      <c r="F18" t="s">
+        <v>202</v>
+      </c>
+      <c r="G18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>2020</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19">
+        <v>2015</v>
+      </c>
+      <c r="E19">
+        <v>152</v>
+      </c>
+      <c r="F19" t="s">
+        <v>202</v>
+      </c>
+      <c r="G19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98C7A7F-43E6-E642-9F02-ED0DAC40D0AF}">
   <dimension ref="A1:F1037"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
@@ -71107,7 +73625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DEA52A-DD20-5F43-9CC3-3845584BAF4F}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -71170,7 +73688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CED1427-52C6-644B-BCE1-B4BE9D18E414}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -71204,119 +73722,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E93042-7294-BF4C-AE0A-DBD708DEC29E}">
-  <dimension ref="A1:A20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>